<commit_message>
Add variable for number of no-go errors across all blocks
</commit_message>
<xml_diff>
--- a/data/variable-legend.xlsx
+++ b/data/variable-legend.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="231">
   <si>
     <t>Table 1</t>
   </si>
@@ -173,6 +173,12 @@
     <t>Proportion of no-go errors for block trials</t>
   </si>
   <si>
+    <t>blkN_nogo_num_errors</t>
+  </si>
+  <si>
+    <t>Number of no-go errors for block trials</t>
+  </si>
+  <si>
     <t>blkN_nogo_next4_avg</t>
   </si>
   <si>
@@ -288,6 +294,12 @@
   </si>
   <si>
     <t>Weighted average reaction time for valid trials preceding each no-go error across all blocks</t>
+  </si>
+  <si>
+    <t>nogo_num_errors</t>
+  </si>
+  <si>
+    <t>Number of no-go errors across all blocks</t>
   </si>
   <si>
     <t>peak_discomfort</t>
@@ -2147,7 +2159,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2451,27 +2463,27 @@
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" ht="27" customHeight="1">
+    <row r="27" ht="15" customHeight="1">
       <c r="A27" t="s" s="12">
         <v>53</v>
       </c>
       <c r="B27" t="s" s="13">
         <v>54</v>
       </c>
-      <c r="C27" t="s" s="14">
-        <v>55</v>
-      </c>
+      <c r="C27" s="14"/>
       <c r="D27" s="7"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" ht="27" customHeight="1">
       <c r="A28" t="s" s="12">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s" s="13">
         <v>56</v>
       </c>
-      <c r="B28" t="s" s="13">
+      <c r="C28" t="s" s="14">
         <v>57</v>
       </c>
-      <c r="C28" s="15"/>
       <c r="D28" s="7"/>
       <c r="E28" s="8"/>
     </row>
@@ -2482,7 +2494,7 @@
       <c r="B29" t="s" s="13">
         <v>59</v>
       </c>
-      <c r="C29" s="14"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="7"/>
       <c r="E29" s="8"/>
     </row>
@@ -2493,20 +2505,20 @@
       <c r="B30" t="s" s="13">
         <v>61</v>
       </c>
-      <c r="C30" t="s" s="14">
-        <v>55</v>
-      </c>
+      <c r="C30" s="14"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" ht="15" customHeight="1">
+    <row r="31" ht="27" customHeight="1">
       <c r="A31" t="s" s="12">
         <v>62</v>
       </c>
       <c r="B31" t="s" s="13">
         <v>63</v>
       </c>
-      <c r="C31" s="14"/>
+      <c r="C31" t="s" s="14">
+        <v>57</v>
+      </c>
       <c r="D31" s="7"/>
       <c r="E31" s="8"/>
     </row>
@@ -2642,7 +2654,7 @@
       <c r="D43" s="7"/>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" ht="27" customHeight="1">
+    <row r="44" ht="15" customHeight="1">
       <c r="A44" t="s" s="12">
         <v>88</v>
       </c>
@@ -2664,40 +2676,38 @@
       <c r="D45" s="7"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" ht="15" customHeight="1">
+    <row r="46" ht="27" customHeight="1">
       <c r="A46" t="s" s="12">
         <v>92</v>
       </c>
       <c r="B46" t="s" s="13">
         <v>93</v>
       </c>
-      <c r="C46" t="s" s="14">
-        <v>94</v>
-      </c>
+      <c r="C46" s="14"/>
       <c r="D46" s="7"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" ht="15" customHeight="1">
       <c r="A47" t="s" s="12">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s" s="13">
         <v>95</v>
       </c>
-      <c r="B47" t="s" s="13">
-        <v>96</v>
-      </c>
-      <c r="C47" t="s" s="14">
-        <v>94</v>
-      </c>
+      <c r="C47" s="14"/>
       <c r="D47" s="7"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" ht="15" customHeight="1">
       <c r="A48" t="s" s="12">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="B48" t="s" s="13">
+      <c r="C48" t="s" s="14">
         <v>98</v>
       </c>
-      <c r="C48" s="14"/>
       <c r="D48" s="7"/>
       <c r="E48" s="8"/>
     </row>
@@ -2708,7 +2718,9 @@
       <c r="B49" t="s" s="13">
         <v>100</v>
       </c>
-      <c r="C49" s="14"/>
+      <c r="C49" t="s" s="14">
+        <v>98</v>
+      </c>
       <c r="D49" s="7"/>
       <c r="E49" s="8"/>
     </row>
@@ -2723,41 +2735,37 @@
       <c r="D50" s="7"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" ht="27" customHeight="1">
+    <row r="51" ht="15" customHeight="1">
       <c r="A51" t="s" s="12">
         <v>103</v>
       </c>
       <c r="B51" t="s" s="13">
         <v>104</v>
       </c>
-      <c r="C51" t="s" s="14">
-        <v>105</v>
-      </c>
+      <c r="C51" s="14"/>
       <c r="D51" s="7"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" ht="15" customHeight="1">
       <c r="A52" t="s" s="12">
+        <v>105</v>
+      </c>
+      <c r="B52" t="s" s="13">
         <v>106</v>
       </c>
-      <c r="B52" t="s" s="13">
-        <v>107</v>
-      </c>
-      <c r="C52" t="s" s="14">
-        <v>105</v>
-      </c>
+      <c r="C52" s="14"/>
       <c r="D52" s="7"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" ht="27" customHeight="1">
       <c r="A53" t="s" s="12">
+        <v>107</v>
+      </c>
+      <c r="B53" t="s" s="13">
         <v>108</v>
       </c>
-      <c r="B53" t="s" s="13">
+      <c r="C53" t="s" s="14">
         <v>109</v>
-      </c>
-      <c r="C53" t="s" s="14">
-        <v>105</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="8"/>
@@ -2770,12 +2778,12 @@
         <v>111</v>
       </c>
       <c r="C54" t="s" s="14">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="8"/>
     </row>
-    <row r="55" ht="15" customHeight="1">
+    <row r="55" ht="27" customHeight="1">
       <c r="A55" t="s" s="12">
         <v>112</v>
       </c>
@@ -2783,7 +2791,7 @@
         <v>113</v>
       </c>
       <c r="C55" t="s" s="14">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="8"/>
@@ -2796,7 +2804,7 @@
         <v>115</v>
       </c>
       <c r="C56" t="s" s="14">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="8"/>
@@ -2809,7 +2817,7 @@
         <v>117</v>
       </c>
       <c r="C57" t="s" s="14">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="8"/>
@@ -2822,7 +2830,7 @@
         <v>119</v>
       </c>
       <c r="C58" t="s" s="14">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="8"/>
@@ -2834,7 +2842,9 @@
       <c r="B59" t="s" s="13">
         <v>121</v>
       </c>
-      <c r="C59" s="15"/>
+      <c r="C59" t="s" s="14">
+        <v>109</v>
+      </c>
       <c r="D59" s="7"/>
       <c r="E59" s="8"/>
     </row>
@@ -2842,11 +2852,11 @@
       <c r="A60" t="s" s="12">
         <v>122</v>
       </c>
-      <c r="B60" t="s" s="16">
-        <v>121</v>
-      </c>
-      <c r="C60" t="s" s="13">
+      <c r="B60" t="s" s="13">
         <v>123</v>
+      </c>
+      <c r="C60" t="s" s="14">
+        <v>109</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="8"/>
@@ -2855,36 +2865,34 @@
       <c r="A61" t="s" s="12">
         <v>124</v>
       </c>
-      <c r="B61" t="s" s="16">
-        <v>121</v>
-      </c>
-      <c r="C61" s="17"/>
+      <c r="B61" t="s" s="13">
+        <v>125</v>
+      </c>
+      <c r="C61" s="15"/>
       <c r="D61" s="7"/>
       <c r="E61" s="8"/>
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="A62" t="s" s="12">
+        <v>126</v>
+      </c>
+      <c r="B62" t="s" s="16">
         <v>125</v>
       </c>
-      <c r="B62" t="s" s="16">
-        <v>121</v>
-      </c>
       <c r="C62" t="s" s="13">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" ht="15" customHeight="1">
       <c r="A63" t="s" s="12">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B63" t="s" s="16">
-        <v>121</v>
-      </c>
-      <c r="C63" t="s" s="13">
-        <v>128</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C63" s="17"/>
       <c r="D63" s="7"/>
       <c r="E63" s="8"/>
     </row>
@@ -2892,10 +2900,10 @@
       <c r="A64" t="s" s="12">
         <v>129</v>
       </c>
-      <c r="B64" t="s" s="13">
-        <v>121</v>
-      </c>
-      <c r="C64" t="s" s="14">
+      <c r="B64" t="s" s="16">
+        <v>125</v>
+      </c>
+      <c r="C64" t="s" s="13">
         <v>130</v>
       </c>
       <c r="D64" s="7"/>
@@ -2905,10 +2913,10 @@
       <c r="A65" t="s" s="12">
         <v>131</v>
       </c>
-      <c r="B65" t="s" s="13">
-        <v>121</v>
-      </c>
-      <c r="C65" t="s" s="14">
+      <c r="B65" t="s" s="16">
+        <v>125</v>
+      </c>
+      <c r="C65" t="s" s="13">
         <v>132</v>
       </c>
       <c r="D65" s="7"/>
@@ -2919,7 +2927,7 @@
         <v>133</v>
       </c>
       <c r="B66" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C66" t="s" s="14">
         <v>134</v>
@@ -2932,7 +2940,7 @@
         <v>135</v>
       </c>
       <c r="B67" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C67" t="s" s="14">
         <v>136</v>
@@ -2945,7 +2953,7 @@
         <v>137</v>
       </c>
       <c r="B68" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C68" t="s" s="14">
         <v>138</v>
@@ -2958,7 +2966,7 @@
         <v>139</v>
       </c>
       <c r="B69" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C69" t="s" s="14">
         <v>140</v>
@@ -2971,7 +2979,7 @@
         <v>141</v>
       </c>
       <c r="B70" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C70" t="s" s="14">
         <v>142</v>
@@ -2984,7 +2992,7 @@
         <v>143</v>
       </c>
       <c r="B71" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C71" t="s" s="14">
         <v>144</v>
@@ -2997,7 +3005,7 @@
         <v>145</v>
       </c>
       <c r="B72" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C72" t="s" s="14">
         <v>146</v>
@@ -3010,7 +3018,7 @@
         <v>147</v>
       </c>
       <c r="B73" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C73" t="s" s="14">
         <v>148</v>
@@ -3023,7 +3031,7 @@
         <v>149</v>
       </c>
       <c r="B74" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C74" t="s" s="14">
         <v>150</v>
@@ -3036,36 +3044,36 @@
         <v>151</v>
       </c>
       <c r="B75" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C75" t="s" s="14">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="8"/>
     </row>
     <row r="76" ht="15" customHeight="1">
       <c r="A76" t="s" s="12">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B76" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C76" t="s" s="14">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="8"/>
     </row>
     <row r="77" ht="15" customHeight="1">
       <c r="A77" t="s" s="12">
+        <v>155</v>
+      </c>
+      <c r="B77" t="s" s="13">
+        <v>125</v>
+      </c>
+      <c r="C77" t="s" s="14">
         <v>154</v>
-      </c>
-      <c r="B77" t="s" s="13">
-        <v>121</v>
-      </c>
-      <c r="C77" t="s" s="14">
-        <v>155</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="8"/>
@@ -3075,7 +3083,7 @@
         <v>156</v>
       </c>
       <c r="B78" t="s" s="13">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C78" t="s" s="14">
         <v>157</v>
@@ -3083,38 +3091,38 @@
       <c r="D78" s="7"/>
       <c r="E78" s="8"/>
     </row>
-    <row r="79" ht="27" customHeight="1">
+    <row r="79" ht="15" customHeight="1">
       <c r="A79" t="s" s="12">
         <v>158</v>
       </c>
       <c r="B79" t="s" s="13">
+        <v>125</v>
+      </c>
+      <c r="C79" t="s" s="14">
         <v>159</v>
-      </c>
-      <c r="C79" t="s" s="14">
-        <v>160</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="8"/>
     </row>
-    <row r="80" ht="27" customHeight="1">
+    <row r="80" ht="15" customHeight="1">
       <c r="A80" t="s" s="12">
+        <v>160</v>
+      </c>
+      <c r="B80" t="s" s="13">
+        <v>125</v>
+      </c>
+      <c r="C80" t="s" s="14">
         <v>161</v>
-      </c>
-      <c r="B80" t="s" s="13">
-        <v>159</v>
-      </c>
-      <c r="C80" t="s" s="14">
-        <v>162</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="8"/>
     </row>
     <row r="81" ht="27" customHeight="1">
       <c r="A81" t="s" s="12">
+        <v>162</v>
+      </c>
+      <c r="B81" t="s" s="13">
         <v>163</v>
-      </c>
-      <c r="B81" t="s" s="13">
-        <v>159</v>
       </c>
       <c r="C81" t="s" s="14">
         <v>164</v>
@@ -3122,12 +3130,12 @@
       <c r="D81" s="7"/>
       <c r="E81" s="8"/>
     </row>
-    <row r="82" ht="39" customHeight="1">
+    <row r="82" ht="27" customHeight="1">
       <c r="A82" t="s" s="12">
         <v>165</v>
       </c>
       <c r="B82" t="s" s="13">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C82" t="s" s="14">
         <v>166</v>
@@ -3135,12 +3143,12 @@
       <c r="D82" s="7"/>
       <c r="E82" s="8"/>
     </row>
-    <row r="83" ht="15" customHeight="1">
+    <row r="83" ht="27" customHeight="1">
       <c r="A83" t="s" s="12">
         <v>167</v>
       </c>
       <c r="B83" t="s" s="13">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C83" t="s" s="14">
         <v>168</v>
@@ -3148,12 +3156,12 @@
       <c r="D83" s="7"/>
       <c r="E83" s="8"/>
     </row>
-    <row r="84" ht="15" customHeight="1">
+    <row r="84" ht="39" customHeight="1">
       <c r="A84" t="s" s="12">
         <v>169</v>
       </c>
       <c r="B84" t="s" s="13">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C84" t="s" s="14">
         <v>170</v>
@@ -3166,7 +3174,7 @@
         <v>171</v>
       </c>
       <c r="B85" t="s" s="13">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C85" t="s" s="14">
         <v>172</v>
@@ -3179,33 +3187,33 @@
         <v>173</v>
       </c>
       <c r="B86" t="s" s="13">
+        <v>163</v>
+      </c>
+      <c r="C86" t="s" s="14">
         <v>174</v>
-      </c>
-      <c r="C86" t="s" s="14">
-        <v>175</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="8"/>
     </row>
-    <row r="87" ht="27" customHeight="1">
+    <row r="87" ht="15" customHeight="1">
       <c r="A87" t="s" s="12">
+        <v>175</v>
+      </c>
+      <c r="B87" t="s" s="13">
+        <v>163</v>
+      </c>
+      <c r="C87" t="s" s="14">
         <v>176</v>
-      </c>
-      <c r="B87" t="s" s="13">
-        <v>174</v>
-      </c>
-      <c r="C87" t="s" s="14">
-        <v>177</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="8"/>
     </row>
-    <row r="88" ht="27" customHeight="1">
+    <row r="88" ht="15" customHeight="1">
       <c r="A88" t="s" s="12">
+        <v>177</v>
+      </c>
+      <c r="B88" t="s" s="13">
         <v>178</v>
-      </c>
-      <c r="B88" t="s" s="13">
-        <v>174</v>
       </c>
       <c r="C88" t="s" s="14">
         <v>179</v>
@@ -3213,12 +3221,12 @@
       <c r="D88" s="7"/>
       <c r="E88" s="8"/>
     </row>
-    <row r="89" ht="15" customHeight="1">
+    <row r="89" ht="27" customHeight="1">
       <c r="A89" t="s" s="12">
         <v>180</v>
       </c>
       <c r="B89" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C89" t="s" s="14">
         <v>181</v>
@@ -3231,7 +3239,7 @@
         <v>182</v>
       </c>
       <c r="B90" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C90" t="s" s="14">
         <v>183</v>
@@ -3244,7 +3252,7 @@
         <v>184</v>
       </c>
       <c r="B91" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C91" t="s" s="14">
         <v>185</v>
@@ -3252,12 +3260,12 @@
       <c r="D91" s="7"/>
       <c r="E91" s="8"/>
     </row>
-    <row r="92" ht="15" customHeight="1">
+    <row r="92" ht="27" customHeight="1">
       <c r="A92" t="s" s="12">
         <v>186</v>
       </c>
       <c r="B92" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C92" t="s" s="14">
         <v>187</v>
@@ -3265,12 +3273,12 @@
       <c r="D92" s="7"/>
       <c r="E92" s="8"/>
     </row>
-    <row r="93" ht="27" customHeight="1">
+    <row r="93" ht="15" customHeight="1">
       <c r="A93" t="s" s="12">
         <v>188</v>
       </c>
       <c r="B93" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C93" t="s" s="14">
         <v>189</v>
@@ -3283,7 +3291,7 @@
         <v>190</v>
       </c>
       <c r="B94" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C94" t="s" s="14">
         <v>191</v>
@@ -3296,7 +3304,7 @@
         <v>192</v>
       </c>
       <c r="B95" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C95" t="s" s="14">
         <v>193</v>
@@ -3304,12 +3312,12 @@
       <c r="D95" s="7"/>
       <c r="E95" s="8"/>
     </row>
-    <row r="96" ht="27" customHeight="1">
+    <row r="96" ht="15" customHeight="1">
       <c r="A96" t="s" s="12">
         <v>194</v>
       </c>
       <c r="B96" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C96" t="s" s="14">
         <v>195</v>
@@ -3317,12 +3325,12 @@
       <c r="D96" s="7"/>
       <c r="E96" s="8"/>
     </row>
-    <row r="97" ht="15" customHeight="1">
+    <row r="97" ht="27" customHeight="1">
       <c r="A97" t="s" s="12">
         <v>196</v>
       </c>
       <c r="B97" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C97" t="s" s="14">
         <v>197</v>
@@ -3330,12 +3338,12 @@
       <c r="D97" s="7"/>
       <c r="E97" s="8"/>
     </row>
-    <row r="98" ht="15" customHeight="1">
+    <row r="98" ht="27" customHeight="1">
       <c r="A98" t="s" s="12">
         <v>198</v>
       </c>
       <c r="B98" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C98" t="s" s="14">
         <v>199</v>
@@ -3348,7 +3356,7 @@
         <v>200</v>
       </c>
       <c r="B99" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C99" t="s" s="14">
         <v>201</v>
@@ -3361,7 +3369,7 @@
         <v>202</v>
       </c>
       <c r="B100" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C100" t="s" s="14">
         <v>203</v>
@@ -3369,12 +3377,12 @@
       <c r="D100" s="7"/>
       <c r="E100" s="8"/>
     </row>
-    <row r="101" ht="27" customHeight="1">
+    <row r="101" ht="15" customHeight="1">
       <c r="A101" t="s" s="12">
         <v>204</v>
       </c>
       <c r="B101" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C101" t="s" s="14">
         <v>205</v>
@@ -3382,12 +3390,12 @@
       <c r="D101" s="7"/>
       <c r="E101" s="8"/>
     </row>
-    <row r="102" ht="27" customHeight="1">
+    <row r="102" ht="15" customHeight="1">
       <c r="A102" t="s" s="12">
         <v>206</v>
       </c>
       <c r="B102" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C102" t="s" s="14">
         <v>207</v>
@@ -3395,12 +3403,12 @@
       <c r="D102" s="7"/>
       <c r="E102" s="8"/>
     </row>
-    <row r="103" ht="15" customHeight="1">
+    <row r="103" ht="27" customHeight="1">
       <c r="A103" t="s" s="12">
         <v>208</v>
       </c>
       <c r="B103" t="s" s="13">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C103" t="s" s="14">
         <v>209</v>
@@ -3413,33 +3421,33 @@
         <v>210</v>
       </c>
       <c r="B104" t="s" s="13">
+        <v>178</v>
+      </c>
+      <c r="C104" t="s" s="14">
         <v>211</v>
-      </c>
-      <c r="C104" t="s" s="14">
-        <v>212</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="8"/>
     </row>
-    <row r="105" ht="27" customHeight="1">
+    <row r="105" ht="15" customHeight="1">
       <c r="A105" t="s" s="12">
+        <v>212</v>
+      </c>
+      <c r="B105" t="s" s="13">
+        <v>178</v>
+      </c>
+      <c r="C105" t="s" s="14">
         <v>213</v>
-      </c>
-      <c r="B105" t="s" s="13">
-        <v>211</v>
-      </c>
-      <c r="C105" t="s" s="14">
-        <v>214</v>
       </c>
       <c r="D105" s="7"/>
       <c r="E105" s="8"/>
     </row>
-    <row r="106" ht="15" customHeight="1">
+    <row r="106" ht="27" customHeight="1">
       <c r="A106" t="s" s="12">
+        <v>214</v>
+      </c>
+      <c r="B106" t="s" s="13">
         <v>215</v>
-      </c>
-      <c r="B106" t="s" s="13">
-        <v>211</v>
       </c>
       <c r="C106" t="s" s="14">
         <v>216</v>
@@ -3452,7 +3460,7 @@
         <v>217</v>
       </c>
       <c r="B107" t="s" s="13">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C107" t="s" s="14">
         <v>218</v>
@@ -3460,12 +3468,12 @@
       <c r="D107" s="7"/>
       <c r="E107" s="8"/>
     </row>
-    <row r="108" ht="27" customHeight="1">
+    <row r="108" ht="15" customHeight="1">
       <c r="A108" t="s" s="12">
         <v>219</v>
       </c>
       <c r="B108" t="s" s="13">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C108" t="s" s="14">
         <v>220</v>
@@ -3478,7 +3486,7 @@
         <v>221</v>
       </c>
       <c r="B109" t="s" s="13">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C109" t="s" s="14">
         <v>222</v>
@@ -3491,7 +3499,7 @@
         <v>223</v>
       </c>
       <c r="B110" t="s" s="13">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C110" t="s" s="14">
         <v>224</v>
@@ -3504,13 +3512,39 @@
         <v>225</v>
       </c>
       <c r="B111" t="s" s="13">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C111" t="s" s="14">
         <v>226</v>
       </c>
-      <c r="D111" s="18"/>
-      <c r="E111" s="19"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="8"/>
+    </row>
+    <row r="112" ht="27" customHeight="1">
+      <c r="A112" t="s" s="12">
+        <v>227</v>
+      </c>
+      <c r="B112" t="s" s="13">
+        <v>215</v>
+      </c>
+      <c r="C112" t="s" s="14">
+        <v>228</v>
+      </c>
+      <c r="D112" s="7"/>
+      <c r="E112" s="8"/>
+    </row>
+    <row r="113" ht="27" customHeight="1">
+      <c r="A113" t="s" s="12">
+        <v>229</v>
+      </c>
+      <c r="B113" t="s" s="13">
+        <v>215</v>
+      </c>
+      <c r="C113" t="s" s="14">
+        <v>230</v>
+      </c>
+      <c r="D113" s="18"/>
+      <c r="E113" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update variable legend with new vars
</commit_message>
<xml_diff>
--- a/data/variable-legend.xlsx
+++ b/data/variable-legend.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="243">
   <si>
     <t>Table 1</t>
   </si>
@@ -315,6 +315,42 @@
   </si>
   <si>
     <t>Peak effort rating</t>
+  </si>
+  <si>
+    <t>prop_discomfort_downs</t>
+  </si>
+  <si>
+    <t>Proportion of discomfort ratings that dropped from the previous discomfort rating</t>
+  </si>
+  <si>
+    <t>prop_discomfort_sames</t>
+  </si>
+  <si>
+    <t>Proportion of discomfort ratings that held steady with the previous discomfort rating</t>
+  </si>
+  <si>
+    <t>prop_discomfort_ups</t>
+  </si>
+  <si>
+    <t>Proportion of discomfort ratings that increased from the previous discomfort rating</t>
+  </si>
+  <si>
+    <t>prop_effort_downs</t>
+  </si>
+  <si>
+    <t>Proportion of effort ratings that dropped from the previous effort rating</t>
+  </si>
+  <si>
+    <t>prop_effort_sames</t>
+  </si>
+  <si>
+    <t>Proportion of effort ratings that held steady with the previous effort rating</t>
+  </si>
+  <si>
+    <t>prop_effort_ups</t>
+  </si>
+  <si>
+    <t>Proportion of effort ratings that increased from the previous effort rating</t>
   </si>
   <si>
     <t>start_accuracy</t>
@@ -2159,7 +2195,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2724,7 +2760,7 @@
       <c r="D49" s="7"/>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" ht="15" customHeight="1">
+    <row r="50" ht="27" customHeight="1">
       <c r="A50" t="s" s="12">
         <v>101</v>
       </c>
@@ -2735,7 +2771,7 @@
       <c r="D50" s="7"/>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" ht="15" customHeight="1">
+    <row r="51" ht="27" customHeight="1">
       <c r="A51" t="s" s="12">
         <v>103</v>
       </c>
@@ -2746,7 +2782,7 @@
       <c r="D51" s="7"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" ht="15" customHeight="1">
+    <row r="52" ht="27" customHeight="1">
       <c r="A52" t="s" s="12">
         <v>105</v>
       </c>
@@ -2764,86 +2800,74 @@
       <c r="B53" t="s" s="13">
         <v>108</v>
       </c>
-      <c r="C53" t="s" s="14">
-        <v>109</v>
-      </c>
+      <c r="C53" s="14"/>
       <c r="D53" s="7"/>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" ht="15" customHeight="1">
+    <row r="54" ht="27" customHeight="1">
       <c r="A54" t="s" s="12">
+        <v>109</v>
+      </c>
+      <c r="B54" t="s" s="13">
         <v>110</v>
       </c>
-      <c r="B54" t="s" s="13">
-        <v>111</v>
-      </c>
-      <c r="C54" t="s" s="14">
-        <v>109</v>
-      </c>
+      <c r="C54" s="14"/>
       <c r="D54" s="7"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" ht="27" customHeight="1">
       <c r="A55" t="s" s="12">
+        <v>111</v>
+      </c>
+      <c r="B55" t="s" s="13">
         <v>112</v>
       </c>
-      <c r="B55" t="s" s="13">
-        <v>113</v>
-      </c>
-      <c r="C55" t="s" s="14">
-        <v>109</v>
-      </c>
+      <c r="C55" s="14"/>
       <c r="D55" s="7"/>
       <c r="E55" s="8"/>
     </row>
     <row r="56" ht="15" customHeight="1">
       <c r="A56" t="s" s="12">
+        <v>113</v>
+      </c>
+      <c r="B56" t="s" s="13">
         <v>114</v>
       </c>
-      <c r="B56" t="s" s="13">
-        <v>115</v>
-      </c>
-      <c r="C56" t="s" s="14">
-        <v>109</v>
-      </c>
+      <c r="C56" s="14"/>
       <c r="D56" s="7"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" t="s" s="12">
+        <v>115</v>
+      </c>
+      <c r="B57" t="s" s="13">
         <v>116</v>
       </c>
-      <c r="B57" t="s" s="13">
-        <v>117</v>
-      </c>
-      <c r="C57" t="s" s="14">
-        <v>109</v>
-      </c>
+      <c r="C57" s="14"/>
       <c r="D57" s="7"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" ht="15" customHeight="1">
       <c r="A58" t="s" s="12">
+        <v>117</v>
+      </c>
+      <c r="B58" t="s" s="13">
         <v>118</v>
       </c>
-      <c r="B58" t="s" s="13">
-        <v>119</v>
-      </c>
-      <c r="C58" t="s" s="14">
-        <v>109</v>
-      </c>
+      <c r="C58" s="14"/>
       <c r="D58" s="7"/>
       <c r="E58" s="8"/>
     </row>
-    <row r="59" ht="15" customHeight="1">
+    <row r="59" ht="27" customHeight="1">
       <c r="A59" t="s" s="12">
+        <v>119</v>
+      </c>
+      <c r="B59" t="s" s="13">
         <v>120</v>
       </c>
-      <c r="B59" t="s" s="13">
+      <c r="C59" t="s" s="14">
         <v>121</v>
-      </c>
-      <c r="C59" t="s" s="14">
-        <v>109</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="8"/>
@@ -2856,19 +2880,21 @@
         <v>123</v>
       </c>
       <c r="C60" t="s" s="14">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="8"/>
     </row>
-    <row r="61" ht="15" customHeight="1">
+    <row r="61" ht="27" customHeight="1">
       <c r="A61" t="s" s="12">
         <v>124</v>
       </c>
       <c r="B61" t="s" s="13">
         <v>125</v>
       </c>
-      <c r="C61" s="15"/>
+      <c r="C61" t="s" s="14">
+        <v>121</v>
+      </c>
       <c r="D61" s="7"/>
       <c r="E61" s="8"/>
     </row>
@@ -2876,11 +2902,11 @@
       <c r="A62" t="s" s="12">
         <v>126</v>
       </c>
-      <c r="B62" t="s" s="16">
-        <v>125</v>
-      </c>
-      <c r="C62" t="s" s="13">
+      <c r="B62" t="s" s="13">
         <v>127</v>
+      </c>
+      <c r="C62" t="s" s="14">
+        <v>121</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="8"/>
@@ -2889,88 +2915,86 @@
       <c r="A63" t="s" s="12">
         <v>128</v>
       </c>
-      <c r="B63" t="s" s="16">
-        <v>125</v>
-      </c>
-      <c r="C63" s="17"/>
+      <c r="B63" t="s" s="13">
+        <v>129</v>
+      </c>
+      <c r="C63" t="s" s="14">
+        <v>121</v>
+      </c>
       <c r="D63" s="7"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" ht="15" customHeight="1">
       <c r="A64" t="s" s="12">
-        <v>129</v>
-      </c>
-      <c r="B64" t="s" s="16">
-        <v>125</v>
-      </c>
-      <c r="C64" t="s" s="13">
         <v>130</v>
+      </c>
+      <c r="B64" t="s" s="13">
+        <v>131</v>
+      </c>
+      <c r="C64" t="s" s="14">
+        <v>121</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" ht="15" customHeight="1">
       <c r="A65" t="s" s="12">
-        <v>131</v>
-      </c>
-      <c r="B65" t="s" s="16">
-        <v>125</v>
-      </c>
-      <c r="C65" t="s" s="13">
         <v>132</v>
+      </c>
+      <c r="B65" t="s" s="13">
+        <v>133</v>
+      </c>
+      <c r="C65" t="s" s="14">
+        <v>121</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" ht="15" customHeight="1">
       <c r="A66" t="s" s="12">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s" s="13">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C66" t="s" s="14">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="8"/>
     </row>
     <row r="67" ht="15" customHeight="1">
       <c r="A67" t="s" s="12">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B67" t="s" s="13">
-        <v>125</v>
-      </c>
-      <c r="C67" t="s" s="14">
-        <v>136</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="C67" s="15"/>
       <c r="D67" s="7"/>
       <c r="E67" s="8"/>
     </row>
     <row r="68" ht="15" customHeight="1">
       <c r="A68" t="s" s="12">
+        <v>138</v>
+      </c>
+      <c r="B68" t="s" s="16">
         <v>137</v>
       </c>
-      <c r="B68" t="s" s="13">
-        <v>125</v>
-      </c>
-      <c r="C68" t="s" s="14">
-        <v>138</v>
+      <c r="C68" t="s" s="13">
+        <v>139</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="8"/>
     </row>
     <row r="69" ht="15" customHeight="1">
       <c r="A69" t="s" s="12">
-        <v>139</v>
-      </c>
-      <c r="B69" t="s" s="13">
-        <v>125</v>
-      </c>
-      <c r="C69" t="s" s="14">
         <v>140</v>
       </c>
+      <c r="B69" t="s" s="16">
+        <v>137</v>
+      </c>
+      <c r="C69" s="17"/>
       <c r="D69" s="7"/>
       <c r="E69" s="8"/>
     </row>
@@ -2978,10 +3002,10 @@
       <c r="A70" t="s" s="12">
         <v>141</v>
       </c>
-      <c r="B70" t="s" s="13">
-        <v>125</v>
-      </c>
-      <c r="C70" t="s" s="14">
+      <c r="B70" t="s" s="16">
+        <v>137</v>
+      </c>
+      <c r="C70" t="s" s="13">
         <v>142</v>
       </c>
       <c r="D70" s="7"/>
@@ -2991,10 +3015,10 @@
       <c r="A71" t="s" s="12">
         <v>143</v>
       </c>
-      <c r="B71" t="s" s="13">
-        <v>125</v>
-      </c>
-      <c r="C71" t="s" s="14">
+      <c r="B71" t="s" s="16">
+        <v>137</v>
+      </c>
+      <c r="C71" t="s" s="13">
         <v>144</v>
       </c>
       <c r="D71" s="7"/>
@@ -3005,7 +3029,7 @@
         <v>145</v>
       </c>
       <c r="B72" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C72" t="s" s="14">
         <v>146</v>
@@ -3018,7 +3042,7 @@
         <v>147</v>
       </c>
       <c r="B73" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C73" t="s" s="14">
         <v>148</v>
@@ -3031,7 +3055,7 @@
         <v>149</v>
       </c>
       <c r="B74" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C74" t="s" s="14">
         <v>150</v>
@@ -3044,7 +3068,7 @@
         <v>151</v>
       </c>
       <c r="B75" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C75" t="s" s="14">
         <v>152</v>
@@ -3057,7 +3081,7 @@
         <v>153</v>
       </c>
       <c r="B76" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C76" t="s" s="14">
         <v>154</v>
@@ -3070,59 +3094,59 @@
         <v>155</v>
       </c>
       <c r="B77" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C77" t="s" s="14">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="8"/>
     </row>
     <row r="78" ht="15" customHeight="1">
       <c r="A78" t="s" s="12">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C78" t="s" s="14">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="8"/>
     </row>
     <row r="79" ht="15" customHeight="1">
       <c r="A79" t="s" s="12">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B79" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s" s="14">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="8"/>
     </row>
     <row r="80" ht="15" customHeight="1">
       <c r="A80" t="s" s="12">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B80" t="s" s="13">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="C80" t="s" s="14">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D80" s="7"/>
       <c r="E80" s="8"/>
     </row>
-    <row r="81" ht="27" customHeight="1">
+    <row r="81" ht="15" customHeight="1">
       <c r="A81" t="s" s="12">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B81" t="s" s="13">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C81" t="s" s="14">
         <v>164</v>
@@ -3130,12 +3154,12 @@
       <c r="D81" s="7"/>
       <c r="E81" s="8"/>
     </row>
-    <row r="82" ht="27" customHeight="1">
+    <row r="82" ht="15" customHeight="1">
       <c r="A82" t="s" s="12">
         <v>165</v>
       </c>
       <c r="B82" t="s" s="13">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C82" t="s" s="14">
         <v>166</v>
@@ -3143,64 +3167,64 @@
       <c r="D82" s="7"/>
       <c r="E82" s="8"/>
     </row>
-    <row r="83" ht="27" customHeight="1">
+    <row r="83" ht="15" customHeight="1">
       <c r="A83" t="s" s="12">
         <v>167</v>
       </c>
       <c r="B83" t="s" s="13">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="C83" t="s" s="14">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="8"/>
     </row>
-    <row r="84" ht="39" customHeight="1">
+    <row r="84" ht="15" customHeight="1">
       <c r="A84" t="s" s="12">
+        <v>168</v>
+      </c>
+      <c r="B84" t="s" s="13">
+        <v>137</v>
+      </c>
+      <c r="C84" t="s" s="14">
         <v>169</v>
-      </c>
-      <c r="B84" t="s" s="13">
-        <v>163</v>
-      </c>
-      <c r="C84" t="s" s="14">
-        <v>170</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="8"/>
     </row>
     <row r="85" ht="15" customHeight="1">
       <c r="A85" t="s" s="12">
+        <v>170</v>
+      </c>
+      <c r="B85" t="s" s="13">
+        <v>137</v>
+      </c>
+      <c r="C85" t="s" s="14">
         <v>171</v>
-      </c>
-      <c r="B85" t="s" s="13">
-        <v>163</v>
-      </c>
-      <c r="C85" t="s" s="14">
-        <v>172</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="8"/>
     </row>
     <row r="86" ht="15" customHeight="1">
       <c r="A86" t="s" s="12">
+        <v>172</v>
+      </c>
+      <c r="B86" t="s" s="13">
+        <v>137</v>
+      </c>
+      <c r="C86" t="s" s="14">
         <v>173</v>
-      </c>
-      <c r="B86" t="s" s="13">
-        <v>163</v>
-      </c>
-      <c r="C86" t="s" s="14">
-        <v>174</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="8"/>
     </row>
-    <row r="87" ht="15" customHeight="1">
+    <row r="87" ht="27" customHeight="1">
       <c r="A87" t="s" s="12">
+        <v>174</v>
+      </c>
+      <c r="B87" t="s" s="13">
         <v>175</v>
-      </c>
-      <c r="B87" t="s" s="13">
-        <v>163</v>
       </c>
       <c r="C87" t="s" s="14">
         <v>176</v>
@@ -3208,90 +3232,90 @@
       <c r="D87" s="7"/>
       <c r="E87" s="8"/>
     </row>
-    <row r="88" ht="15" customHeight="1">
+    <row r="88" ht="27" customHeight="1">
       <c r="A88" t="s" s="12">
         <v>177</v>
       </c>
       <c r="B88" t="s" s="13">
+        <v>175</v>
+      </c>
+      <c r="C88" t="s" s="14">
         <v>178</v>
-      </c>
-      <c r="C88" t="s" s="14">
-        <v>179</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="8"/>
     </row>
     <row r="89" ht="27" customHeight="1">
       <c r="A89" t="s" s="12">
+        <v>179</v>
+      </c>
+      <c r="B89" t="s" s="13">
+        <v>175</v>
+      </c>
+      <c r="C89" t="s" s="14">
         <v>180</v>
-      </c>
-      <c r="B89" t="s" s="13">
-        <v>178</v>
-      </c>
-      <c r="C89" t="s" s="14">
-        <v>181</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="8"/>
     </row>
-    <row r="90" ht="27" customHeight="1">
+    <row r="90" ht="39" customHeight="1">
       <c r="A90" t="s" s="12">
+        <v>181</v>
+      </c>
+      <c r="B90" t="s" s="13">
+        <v>175</v>
+      </c>
+      <c r="C90" t="s" s="14">
         <v>182</v>
-      </c>
-      <c r="B90" t="s" s="13">
-        <v>178</v>
-      </c>
-      <c r="C90" t="s" s="14">
-        <v>183</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="8"/>
     </row>
     <row r="91" ht="15" customHeight="1">
       <c r="A91" t="s" s="12">
+        <v>183</v>
+      </c>
+      <c r="B91" t="s" s="13">
+        <v>175</v>
+      </c>
+      <c r="C91" t="s" s="14">
         <v>184</v>
-      </c>
-      <c r="B91" t="s" s="13">
-        <v>178</v>
-      </c>
-      <c r="C91" t="s" s="14">
-        <v>185</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="8"/>
     </row>
-    <row r="92" ht="27" customHeight="1">
+    <row r="92" ht="15" customHeight="1">
       <c r="A92" t="s" s="12">
+        <v>185</v>
+      </c>
+      <c r="B92" t="s" s="13">
+        <v>175</v>
+      </c>
+      <c r="C92" t="s" s="14">
         <v>186</v>
-      </c>
-      <c r="B92" t="s" s="13">
-        <v>178</v>
-      </c>
-      <c r="C92" t="s" s="14">
-        <v>187</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="8"/>
     </row>
     <row r="93" ht="15" customHeight="1">
       <c r="A93" t="s" s="12">
+        <v>187</v>
+      </c>
+      <c r="B93" t="s" s="13">
+        <v>175</v>
+      </c>
+      <c r="C93" t="s" s="14">
         <v>188</v>
-      </c>
-      <c r="B93" t="s" s="13">
-        <v>178</v>
-      </c>
-      <c r="C93" t="s" s="14">
-        <v>189</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="8"/>
     </row>
     <row r="94" ht="15" customHeight="1">
       <c r="A94" t="s" s="12">
+        <v>189</v>
+      </c>
+      <c r="B94" t="s" s="13">
         <v>190</v>
-      </c>
-      <c r="B94" t="s" s="13">
-        <v>178</v>
       </c>
       <c r="C94" t="s" s="14">
         <v>191</v>
@@ -3304,7 +3328,7 @@
         <v>192</v>
       </c>
       <c r="B95" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C95" t="s" s="14">
         <v>193</v>
@@ -3312,12 +3336,12 @@
       <c r="D95" s="7"/>
       <c r="E95" s="8"/>
     </row>
-    <row r="96" ht="15" customHeight="1">
+    <row r="96" ht="27" customHeight="1">
       <c r="A96" t="s" s="12">
         <v>194</v>
       </c>
       <c r="B96" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C96" t="s" s="14">
         <v>195</v>
@@ -3325,12 +3349,12 @@
       <c r="D96" s="7"/>
       <c r="E96" s="8"/>
     </row>
-    <row r="97" ht="27" customHeight="1">
+    <row r="97" ht="15" customHeight="1">
       <c r="A97" t="s" s="12">
         <v>196</v>
       </c>
       <c r="B97" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C97" t="s" s="14">
         <v>197</v>
@@ -3343,7 +3367,7 @@
         <v>198</v>
       </c>
       <c r="B98" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C98" t="s" s="14">
         <v>199</v>
@@ -3356,7 +3380,7 @@
         <v>200</v>
       </c>
       <c r="B99" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C99" t="s" s="14">
         <v>201</v>
@@ -3369,7 +3393,7 @@
         <v>202</v>
       </c>
       <c r="B100" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C100" t="s" s="14">
         <v>203</v>
@@ -3377,12 +3401,12 @@
       <c r="D100" s="7"/>
       <c r="E100" s="8"/>
     </row>
-    <row r="101" ht="15" customHeight="1">
+    <row r="101" ht="27" customHeight="1">
       <c r="A101" t="s" s="12">
         <v>204</v>
       </c>
       <c r="B101" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C101" t="s" s="14">
         <v>205</v>
@@ -3395,7 +3419,7 @@
         <v>206</v>
       </c>
       <c r="B102" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C102" t="s" s="14">
         <v>207</v>
@@ -3408,7 +3432,7 @@
         <v>208</v>
       </c>
       <c r="B103" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C103" t="s" s="14">
         <v>209</v>
@@ -3421,7 +3445,7 @@
         <v>210</v>
       </c>
       <c r="B104" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C104" t="s" s="14">
         <v>211</v>
@@ -3434,7 +3458,7 @@
         <v>212</v>
       </c>
       <c r="B105" t="s" s="13">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="C105" t="s" s="14">
         <v>213</v>
@@ -3442,90 +3466,90 @@
       <c r="D105" s="7"/>
       <c r="E105" s="8"/>
     </row>
-    <row r="106" ht="27" customHeight="1">
+    <row r="106" ht="15" customHeight="1">
       <c r="A106" t="s" s="12">
         <v>214</v>
       </c>
       <c r="B106" t="s" s="13">
+        <v>190</v>
+      </c>
+      <c r="C106" t="s" s="14">
         <v>215</v>
-      </c>
-      <c r="C106" t="s" s="14">
-        <v>216</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="8"/>
     </row>
-    <row r="107" ht="27" customHeight="1">
+    <row r="107" ht="15" customHeight="1">
       <c r="A107" t="s" s="12">
+        <v>216</v>
+      </c>
+      <c r="B107" t="s" s="13">
+        <v>190</v>
+      </c>
+      <c r="C107" t="s" s="14">
         <v>217</v>
-      </c>
-      <c r="B107" t="s" s="13">
-        <v>215</v>
-      </c>
-      <c r="C107" t="s" s="14">
-        <v>218</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="8"/>
     </row>
     <row r="108" ht="15" customHeight="1">
       <c r="A108" t="s" s="12">
+        <v>218</v>
+      </c>
+      <c r="B108" t="s" s="13">
+        <v>190</v>
+      </c>
+      <c r="C108" t="s" s="14">
         <v>219</v>
-      </c>
-      <c r="B108" t="s" s="13">
-        <v>215</v>
-      </c>
-      <c r="C108" t="s" s="14">
-        <v>220</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="8"/>
     </row>
     <row r="109" ht="27" customHeight="1">
       <c r="A109" t="s" s="12">
+        <v>220</v>
+      </c>
+      <c r="B109" t="s" s="13">
+        <v>190</v>
+      </c>
+      <c r="C109" t="s" s="14">
         <v>221</v>
-      </c>
-      <c r="B109" t="s" s="13">
-        <v>215</v>
-      </c>
-      <c r="C109" t="s" s="14">
-        <v>222</v>
       </c>
       <c r="D109" s="7"/>
       <c r="E109" s="8"/>
     </row>
     <row r="110" ht="27" customHeight="1">
       <c r="A110" t="s" s="12">
+        <v>222</v>
+      </c>
+      <c r="B110" t="s" s="13">
+        <v>190</v>
+      </c>
+      <c r="C110" t="s" s="14">
         <v>223</v>
-      </c>
-      <c r="B110" t="s" s="13">
-        <v>215</v>
-      </c>
-      <c r="C110" t="s" s="14">
-        <v>224</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="8"/>
     </row>
-    <row r="111" ht="27" customHeight="1">
+    <row r="111" ht="15" customHeight="1">
       <c r="A111" t="s" s="12">
+        <v>224</v>
+      </c>
+      <c r="B111" t="s" s="13">
+        <v>190</v>
+      </c>
+      <c r="C111" t="s" s="14">
         <v>225</v>
-      </c>
-      <c r="B111" t="s" s="13">
-        <v>215</v>
-      </c>
-      <c r="C111" t="s" s="14">
-        <v>226</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="8"/>
     </row>
     <row r="112" ht="27" customHeight="1">
       <c r="A112" t="s" s="12">
+        <v>226</v>
+      </c>
+      <c r="B112" t="s" s="13">
         <v>227</v>
-      </c>
-      <c r="B112" t="s" s="13">
-        <v>215</v>
       </c>
       <c r="C112" t="s" s="14">
         <v>228</v>
@@ -3538,13 +3562,91 @@
         <v>229</v>
       </c>
       <c r="B113" t="s" s="13">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="C113" t="s" s="14">
         <v>230</v>
       </c>
-      <c r="D113" s="18"/>
-      <c r="E113" s="19"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="8"/>
+    </row>
+    <row r="114" ht="15" customHeight="1">
+      <c r="A114" t="s" s="12">
+        <v>231</v>
+      </c>
+      <c r="B114" t="s" s="13">
+        <v>227</v>
+      </c>
+      <c r="C114" t="s" s="14">
+        <v>232</v>
+      </c>
+      <c r="D114" s="7"/>
+      <c r="E114" s="8"/>
+    </row>
+    <row r="115" ht="27" customHeight="1">
+      <c r="A115" t="s" s="12">
+        <v>233</v>
+      </c>
+      <c r="B115" t="s" s="13">
+        <v>227</v>
+      </c>
+      <c r="C115" t="s" s="14">
+        <v>234</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="8"/>
+    </row>
+    <row r="116" ht="27" customHeight="1">
+      <c r="A116" t="s" s="12">
+        <v>235</v>
+      </c>
+      <c r="B116" t="s" s="13">
+        <v>227</v>
+      </c>
+      <c r="C116" t="s" s="14">
+        <v>236</v>
+      </c>
+      <c r="D116" s="7"/>
+      <c r="E116" s="8"/>
+    </row>
+    <row r="117" ht="27" customHeight="1">
+      <c r="A117" t="s" s="12">
+        <v>237</v>
+      </c>
+      <c r="B117" t="s" s="13">
+        <v>227</v>
+      </c>
+      <c r="C117" t="s" s="14">
+        <v>238</v>
+      </c>
+      <c r="D117" s="7"/>
+      <c r="E117" s="8"/>
+    </row>
+    <row r="118" ht="27" customHeight="1">
+      <c r="A118" t="s" s="12">
+        <v>239</v>
+      </c>
+      <c r="B118" t="s" s="13">
+        <v>227</v>
+      </c>
+      <c r="C118" t="s" s="14">
+        <v>240</v>
+      </c>
+      <c r="D118" s="7"/>
+      <c r="E118" s="8"/>
+    </row>
+    <row r="119" ht="27" customHeight="1">
+      <c r="A119" t="s" s="12">
+        <v>241</v>
+      </c>
+      <c r="B119" t="s" s="13">
+        <v>227</v>
+      </c>
+      <c r="C119" t="s" s="14">
+        <v>242</v>
+      </c>
+      <c r="D119" s="18"/>
+      <c r="E119" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update anticipation questions compilation
- Fix compilation ordering
- Update variable legend
</commit_message>
<xml_diff>
--- a/data/variable-legend.xlsx
+++ b/data/variable-legend.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr date1904="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <workbookPr date1904="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="5440" yWindow="1460" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="271">
   <si>
     <t>Table 1</t>
   </si>
@@ -819,16 +826,19 @@
   </si>
   <si>
     <t>Considering the attention task in its entirety: How much enjoyment did you experience?</t>
+  </si>
+  <si>
+    <t>antecedent_boredom</t>
+  </si>
+  <si>
+    <t>Boredom rating prior to experiment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -840,14 +850,21 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="13"/>
+      <b/>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <u/>
       <sz val="10"/>
-      <color indexed="8"/>
+      <color theme="10"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Helvetica"/>
     </font>
   </fonts>
@@ -1110,108 +1127,165 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="22">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -1337,7 +1411,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1346,7 +1420,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1355,7 +1429,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -1429,7 +1503,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -1437,7 +1511,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1456,7 +1530,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1486,7 +1560,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1512,7 +1586,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1538,7 +1612,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1564,7 +1638,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1590,7 +1664,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1616,7 +1690,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1642,7 +1716,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1668,7 +1742,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1694,7 +1768,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1707,9 +1781,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1724,7 +1804,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -1732,7 +1812,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1751,7 +1831,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1777,7 +1857,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1803,7 +1883,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1829,7 +1909,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1855,7 +1935,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1881,7 +1961,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1907,7 +1987,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1933,7 +2013,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1959,7 +2039,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1985,7 +2065,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1998,9 +2078,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -2014,7 +2100,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2033,7 +2119,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2063,7 +2149,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2089,7 +2175,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2115,7 +2201,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2141,7 +2227,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2167,7 +2253,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2193,7 +2279,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2219,7 +2305,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2245,7 +2331,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2271,7 +2357,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2284,1618 +2370,1641 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E131"/>
+  <dimension ref="A1:IV132"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
-    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1640625" style="1" customWidth="1"/>
+    <col min="4" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:5" ht="17" customHeight="1">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="6">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="9">
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="12">
+      <c r="C3" s="9"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s" s="13">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="12">
+      <c r="C4" s="12"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="13">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="14">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="27" customHeight="1">
-      <c r="A6" t="s" s="12">
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="27" customHeight="1">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s" s="13">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s" s="14">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="12">
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s" s="13">
+      <c r="B7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="12">
+      <c r="C7" s="12"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s" s="13">
+      <c r="B8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="12">
+      <c r="C8" s="12"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" customHeight="1">
+      <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s" s="13">
+      <c r="B9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="12">
+      <c r="C9" s="12"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s" s="13">
+      <c r="B10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="12">
+      <c r="C10" s="12"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" customHeight="1">
+      <c r="A11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s" s="13">
+      <c r="B11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="12">
+      <c r="C11" s="12"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s" s="13">
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="12">
+      <c r="C12" s="12"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B13" t="s" s="13">
+      <c r="B13" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="12">
+      <c r="C13" s="12"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s" s="13">
+      <c r="B14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" ht="27" customHeight="1">
-      <c r="A15" t="s" s="12">
+      <c r="C14" s="12"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="27" customHeight="1">
+      <c r="A15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s" s="13">
+      <c r="B15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" ht="27" customHeight="1">
-      <c r="A16" t="s" s="12">
+      <c r="C15" s="12"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="27" customHeight="1">
+      <c r="A16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s" s="13">
+      <c r="B16" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" ht="27" customHeight="1">
-      <c r="A17" t="s" s="12">
+      <c r="C16" s="12"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" ht="27" customHeight="1">
+      <c r="A17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s" s="13">
+      <c r="B17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="12">
+      <c r="C17" s="12"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1">
+      <c r="A18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s" s="13">
+      <c r="B18" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="12">
+      <c r="C18" s="12"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="A19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s" s="13">
+      <c r="B19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" ht="27" customHeight="1">
-      <c r="A20" t="s" s="12">
+      <c r="C19" s="12"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="27" customHeight="1">
+      <c r="A20" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B20" t="s" s="13">
+      <c r="B20" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" ht="27" customHeight="1">
-      <c r="A21" t="s" s="12">
+      <c r="C20" s="12"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" ht="27" customHeight="1">
+      <c r="A21" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s" s="13">
+      <c r="B21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s" s="14">
+      <c r="C21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="12">
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="A22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B22" t="s" s="13">
+      <c r="B22" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s" s="14">
+      <c r="C22" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" ht="15" customHeight="1">
-      <c r="A23" t="s" s="12">
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s" s="13">
+      <c r="B23" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1">
+      <c r="A24" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B24" t="s" s="13">
+      <c r="B24" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="12">
+      <c r="C24" s="12"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1">
+      <c r="A25" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B25" t="s" s="13">
+      <c r="B25" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" ht="15" customHeight="1">
-      <c r="A26" t="s" s="12">
+      <c r="C25" s="12"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1">
+      <c r="A26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B26" t="s" s="13">
+      <c r="B26" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" ht="15" customHeight="1">
-      <c r="A27" t="s" s="12">
+      <c r="C26" s="12"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1">
+      <c r="A27" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B27" t="s" s="13">
+      <c r="B27" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" ht="15" customHeight="1">
-      <c r="A28" t="s" s="12">
+      <c r="C27" s="12"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1">
+      <c r="A28" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B28" t="s" s="13">
+      <c r="B28" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" ht="15" customHeight="1">
-      <c r="A29" t="s" s="12">
+      <c r="C28" s="12"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1">
+      <c r="A29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B29" t="s" s="13">
+      <c r="B29" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" ht="15" customHeight="1">
-      <c r="A30" t="s" s="12">
+      <c r="C29" s="12"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1">
+      <c r="A30" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B30" t="s" s="13">
+      <c r="B30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" ht="15" customHeight="1">
-      <c r="A31" t="s" s="12">
+      <c r="C30" s="12"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1">
+      <c r="A31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B31" t="s" s="13">
+      <c r="B31" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" ht="27" customHeight="1">
-      <c r="A32" t="s" s="12">
+      <c r="C31" s="12"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:5" ht="27" customHeight="1">
+      <c r="A32" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B32" t="s" s="13">
+      <c r="B32" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s" s="14">
+      <c r="C32" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" ht="27" customHeight="1">
-      <c r="A33" t="s" s="12">
+      <c r="D32" s="5"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" ht="27" customHeight="1">
+      <c r="A33" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B33" t="s" s="13">
+      <c r="B33" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" ht="27" customHeight="1">
-      <c r="A34" t="s" s="12">
+      <c r="C33" s="13"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" ht="27" customHeight="1">
+      <c r="A34" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B34" t="s" s="13">
+      <c r="B34" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" ht="27" customHeight="1">
-      <c r="A35" t="s" s="12">
+      <c r="C34" s="12"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" ht="27" customHeight="1">
+      <c r="A35" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B35" t="s" s="13">
+      <c r="B35" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C35" t="s" s="14">
+      <c r="C35" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" ht="15" customHeight="1">
-      <c r="A36" t="s" s="12">
+      <c r="D35" s="5"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1">
+      <c r="A36" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B36" t="s" s="13">
+      <c r="B36" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" ht="15" customHeight="1">
-      <c r="A37" t="s" s="12">
+      <c r="C36" s="12"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" ht="15" customHeight="1">
+      <c r="A37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B37" t="s" s="13">
+      <c r="B37" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" ht="15" customHeight="1">
-      <c r="A38" t="s" s="12">
+      <c r="C37" s="12"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" ht="15" customHeight="1">
+      <c r="A38" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B38" t="s" s="13">
+      <c r="B38" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" ht="15" customHeight="1">
-      <c r="A39" t="s" s="12">
+      <c r="C38" s="12"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" ht="15" customHeight="1">
+      <c r="A39" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B39" t="s" s="13">
+      <c r="B39" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" ht="15" customHeight="1">
-      <c r="A40" t="s" s="12">
+      <c r="C39" s="12"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" ht="15" customHeight="1">
+      <c r="A40" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B40" t="s" s="13">
+      <c r="B40" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" ht="15" customHeight="1">
-      <c r="A41" t="s" s="12">
+      <c r="C40" s="12"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1">
+      <c r="A41" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="B41" t="s" s="13">
+      <c r="B41" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" ht="15" customHeight="1">
-      <c r="A42" t="s" s="12">
+      <c r="C41" s="12"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1">
+      <c r="A42" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B42" t="s" s="13">
+      <c r="B42" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" ht="15" customHeight="1">
-      <c r="A43" t="s" s="12">
+      <c r="C42" s="12"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1">
+      <c r="A43" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B43" t="s" s="13">
+      <c r="B43" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" ht="15" customHeight="1">
-      <c r="A44" t="s" s="12">
+      <c r="C43" s="12"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" ht="15" customHeight="1">
+      <c r="A44" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B44" t="s" s="13">
+      <c r="B44" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" ht="15" customHeight="1">
-      <c r="A45" t="s" s="12">
+      <c r="C44" s="12"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1">
+      <c r="A45" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B45" t="s" s="13">
+      <c r="B45" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" ht="15" customHeight="1">
-      <c r="A46" t="s" s="12">
+      <c r="C45" s="12"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" ht="15" customHeight="1">
+      <c r="A46" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B46" t="s" s="13">
+      <c r="B46" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" ht="15" customHeight="1">
-      <c r="A47" t="s" s="12">
+      <c r="C46" s="12"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" ht="15" customHeight="1">
+      <c r="A47" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" ht="15" customHeight="1">
+      <c r="A48" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B47" t="s" s="13">
+      <c r="B48" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" ht="15" customHeight="1">
-      <c r="A48" t="s" s="12">
+      <c r="C48" s="12"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" ht="15" customHeight="1">
+      <c r="A49" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B48" t="s" s="13">
+      <c r="B49" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="8"/>
-    </row>
-    <row r="49" ht="27" customHeight="1">
-      <c r="A49" t="s" s="12">
+      <c r="C49" s="12"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" ht="27" customHeight="1">
+      <c r="A50" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B49" t="s" s="13">
+      <c r="B50" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" ht="27" customHeight="1">
-      <c r="A50" t="s" s="12">
+      <c r="C50" s="12"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" ht="27" customHeight="1">
+      <c r="A51" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B50" t="s" s="13">
+      <c r="B51" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" ht="15" customHeight="1">
-      <c r="A51" t="s" s="12">
+      <c r="C51" s="12"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5" ht="15" customHeight="1">
+      <c r="A52" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B51" t="s" s="13">
+      <c r="B52" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" ht="15" customHeight="1">
-      <c r="A52" t="s" s="12">
+      <c r="C52" s="12"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="1:5" ht="15" customHeight="1">
+      <c r="A53" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B52" t="s" s="13">
+      <c r="B53" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C52" t="s" s="14">
+      <c r="C53" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" ht="15" customHeight="1">
-      <c r="A53" t="s" s="12">
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="1:5" ht="15" customHeight="1">
+      <c r="A54" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B53" t="s" s="13">
+      <c r="B54" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C53" t="s" s="14">
+      <c r="C54" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" ht="15" customHeight="1">
-      <c r="A54" t="s" s="12">
+      <c r="D54" s="5"/>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1">
+      <c r="A55" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B54" t="s" s="13">
+      <c r="B55" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="55" ht="15" customHeight="1">
-      <c r="A55" t="s" s="12">
+      <c r="C55" s="14"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="1:5" ht="15" customHeight="1">
+      <c r="A56" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="B55" t="s" s="13">
+      <c r="B56" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="8"/>
-    </row>
-    <row r="56" ht="27" customHeight="1">
-      <c r="A56" t="s" s="12">
+      <c r="C56" s="12"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="1:5" ht="27" customHeight="1">
+      <c r="A57" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B56" t="s" s="13">
+      <c r="B57" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" ht="27" customHeight="1">
-      <c r="A57" t="s" s="12">
+      <c r="C57" s="12"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:5" ht="27" customHeight="1">
+      <c r="A58" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B57" t="s" s="13">
+      <c r="B58" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="8"/>
-    </row>
-    <row r="58" ht="27" customHeight="1">
-      <c r="A58" t="s" s="12">
+      <c r="C58" s="12"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:5" ht="27" customHeight="1">
+      <c r="A59" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B58" t="s" s="13">
+      <c r="B59" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" ht="27" customHeight="1">
-      <c r="A59" t="s" s="12">
+      <c r="C59" s="12"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="1:5" ht="27" customHeight="1">
+      <c r="A60" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B59" t="s" s="13">
+      <c r="B60" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="8"/>
-    </row>
-    <row r="60" ht="27" customHeight="1">
-      <c r="A60" t="s" s="12">
+      <c r="C60" s="12"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="1:5" ht="27" customHeight="1">
+      <c r="A61" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B60" t="s" s="13">
+      <c r="B61" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="8"/>
-    </row>
-    <row r="61" ht="27" customHeight="1">
-      <c r="A61" t="s" s="12">
+      <c r="C61" s="12"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="1:5" ht="27" customHeight="1">
+      <c r="A62" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B61" t="s" s="13">
+      <c r="B62" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" ht="15" customHeight="1">
-      <c r="A62" t="s" s="12">
+      <c r="C62" s="12"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1">
+      <c r="A63" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B62" t="s" s="13">
+      <c r="B63" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="63" ht="15" customHeight="1">
-      <c r="A63" t="s" s="12">
+      <c r="C63" s="12"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="1:5" ht="15" customHeight="1">
+      <c r="A64" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B63" t="s" s="13">
+      <c r="B64" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="C63" s="14"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="8"/>
-    </row>
-    <row r="64" ht="15" customHeight="1">
-      <c r="A64" t="s" s="12">
+      <c r="C64" s="12"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="6"/>
+    </row>
+    <row r="65" spans="1:5" ht="15" customHeight="1">
+      <c r="A65" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="B64" t="s" s="13">
+      <c r="B65" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C64" s="14"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="8"/>
-    </row>
-    <row r="65" ht="15" customHeight="1">
-      <c r="A65" t="s" s="12">
+      <c r="C65" s="12"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="1:5" ht="15" customHeight="1">
+      <c r="A66" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="B65" t="s" s="13">
+      <c r="B66" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="8"/>
-    </row>
-    <row r="66" ht="15" customHeight="1">
-      <c r="A66" t="s" s="12">
+      <c r="C66" s="12"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="1:5" ht="15" customHeight="1">
+      <c r="A67" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B66" t="s" s="13">
+      <c r="B67" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="14"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="8"/>
-    </row>
-    <row r="67" ht="15" customHeight="1">
-      <c r="A67" t="s" s="12">
+      <c r="C67" s="12"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="1:5" ht="15" customHeight="1">
+      <c r="A68" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="B67" t="s" s="13">
+      <c r="B68" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" ht="15" customHeight="1">
-      <c r="A68" t="s" s="12">
+      <c r="C68" s="12"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="1:5" ht="15" customHeight="1">
+      <c r="A69" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B68" t="s" s="13">
+      <c r="B69" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C68" s="14"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" ht="15" customHeight="1">
-      <c r="A69" t="s" s="12">
+      <c r="C69" s="12"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="1:5" ht="15" customHeight="1">
+      <c r="A70" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="B69" t="s" s="13">
+      <c r="B70" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="C69" s="14"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="8"/>
-    </row>
-    <row r="70" ht="15" customHeight="1">
-      <c r="A70" t="s" s="12">
+      <c r="C70" s="12"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:5" ht="15" customHeight="1">
+      <c r="A71" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B70" t="s" s="13">
+      <c r="B71" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C70" s="14"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="8"/>
-    </row>
-    <row r="71" ht="27" customHeight="1">
-      <c r="A71" t="s" s="12">
+      <c r="C71" s="12"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="1:5" ht="27" customHeight="1">
+      <c r="A72" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B71" t="s" s="13">
+      <c r="B72" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="C71" t="s" s="14">
+      <c r="C72" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="8"/>
-    </row>
-    <row r="72" ht="15" customHeight="1">
-      <c r="A72" t="s" s="12">
+      <c r="D72" s="5"/>
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="1:5" ht="15" customHeight="1">
+      <c r="A73" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B72" t="s" s="13">
+      <c r="B73" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="C72" t="s" s="14">
+      <c r="C73" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="8"/>
-    </row>
-    <row r="73" ht="27" customHeight="1">
-      <c r="A73" t="s" s="12">
+      <c r="D73" s="5"/>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="1:5" ht="27" customHeight="1">
+      <c r="A74" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B73" t="s" s="13">
+      <c r="B74" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="C73" t="s" s="14">
+      <c r="C74" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D73" s="7"/>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" ht="15" customHeight="1">
-      <c r="A74" t="s" s="12">
+      <c r="D74" s="5"/>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="1:5" ht="15" customHeight="1">
+      <c r="A75" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B74" t="s" s="13">
+      <c r="B75" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C74" t="s" s="14">
+      <c r="C75" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D74" s="7"/>
-      <c r="E74" s="8"/>
-    </row>
-    <row r="75" ht="15" customHeight="1">
-      <c r="A75" t="s" s="12">
+      <c r="D75" s="5"/>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="1:5" ht="15" customHeight="1">
+      <c r="A76" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B75" t="s" s="13">
+      <c r="B76" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C75" t="s" s="14">
+      <c r="C76" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D75" s="7"/>
-      <c r="E75" s="8"/>
-    </row>
-    <row r="76" ht="15" customHeight="1">
-      <c r="A76" t="s" s="12">
+      <c r="D76" s="5"/>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="1:5" ht="15" customHeight="1">
+      <c r="A77" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B76" t="s" s="13">
+      <c r="B77" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C76" t="s" s="14">
+      <c r="C77" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D76" s="7"/>
-      <c r="E76" s="8"/>
-    </row>
-    <row r="77" ht="15" customHeight="1">
-      <c r="A77" t="s" s="12">
+      <c r="D77" s="5"/>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="1:5" ht="15" customHeight="1">
+      <c r="A78" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B77" t="s" s="13">
+      <c r="B78" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C77" t="s" s="14">
+      <c r="C78" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D77" s="7"/>
-      <c r="E77" s="8"/>
-    </row>
-    <row r="78" ht="15" customHeight="1">
-      <c r="A78" t="s" s="12">
+      <c r="D78" s="5"/>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="1:5" ht="15" customHeight="1">
+      <c r="A79" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B78" t="s" s="13">
+      <c r="B79" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C78" t="s" s="14">
+      <c r="C79" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D78" s="7"/>
-      <c r="E78" s="8"/>
-    </row>
-    <row r="79" ht="15" customHeight="1">
-      <c r="A79" t="s" s="12">
+      <c r="D79" s="5"/>
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="1:5" ht="15" customHeight="1">
+      <c r="A80" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B79" t="s" s="13">
+      <c r="B80" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C79" s="15"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="8"/>
-    </row>
-    <row r="80" ht="15" customHeight="1">
-      <c r="A80" t="s" s="12">
+      <c r="C80" s="13"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="1:5" ht="15" customHeight="1">
+      <c r="A81" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B80" t="s" s="18">
+      <c r="B81" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C80" t="s" s="13">
+      <c r="C81" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D80" s="7"/>
-      <c r="E80" s="8"/>
-    </row>
-    <row r="81" ht="15" customHeight="1">
-      <c r="A81" t="s" s="12">
+      <c r="D81" s="5"/>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" ht="15" customHeight="1">
+      <c r="A82" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="B81" t="s" s="18">
+      <c r="B82" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C81" s="19"/>
-      <c r="D81" s="7"/>
-      <c r="E81" s="8"/>
-    </row>
-    <row r="82" ht="15" customHeight="1">
-      <c r="A82" t="s" s="12">
+      <c r="C82" s="17"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="1:5" ht="15" customHeight="1">
+      <c r="A83" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="B82" t="s" s="18">
+      <c r="B83" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C82" t="s" s="13">
+      <c r="C83" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D82" s="7"/>
-      <c r="E82" s="8"/>
-    </row>
-    <row r="83" ht="15" customHeight="1">
-      <c r="A83" t="s" s="12">
+      <c r="D83" s="5"/>
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="1:5" ht="15" customHeight="1">
+      <c r="A84" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="B83" t="s" s="18">
+      <c r="B84" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C83" t="s" s="13">
+      <c r="C84" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D83" s="7"/>
-      <c r="E83" s="8"/>
-    </row>
-    <row r="84" ht="15" customHeight="1">
-      <c r="A84" t="s" s="12">
+      <c r="D84" s="5"/>
+      <c r="E84" s="6"/>
+    </row>
+    <row r="85" spans="1:5" ht="15" customHeight="1">
+      <c r="A85" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B84" t="s" s="13">
+      <c r="B85" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C84" t="s" s="14">
+      <c r="C85" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="D84" s="7"/>
-      <c r="E84" s="8"/>
-    </row>
-    <row r="85" ht="15" customHeight="1">
-      <c r="A85" t="s" s="12">
+      <c r="D85" s="5"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="1:5" ht="15" customHeight="1">
+      <c r="A86" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B85" t="s" s="13">
+      <c r="B86" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C85" t="s" s="14">
+      <c r="C86" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D85" s="7"/>
-      <c r="E85" s="8"/>
-    </row>
-    <row r="86" ht="15" customHeight="1">
-      <c r="A86" t="s" s="12">
+      <c r="D86" s="5"/>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="1:5" ht="15" customHeight="1">
+      <c r="A87" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="B86" t="s" s="13">
+      <c r="B87" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C86" t="s" s="14">
+      <c r="C87" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D86" s="7"/>
-      <c r="E86" s="8"/>
-    </row>
-    <row r="87" ht="15" customHeight="1">
-      <c r="A87" t="s" s="12">
+      <c r="D87" s="5"/>
+      <c r="E87" s="6"/>
+    </row>
+    <row r="88" spans="1:5" ht="15" customHeight="1">
+      <c r="A88" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B87" t="s" s="13">
+      <c r="B88" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C87" t="s" s="14">
+      <c r="C88" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D87" s="7"/>
-      <c r="E87" s="8"/>
-    </row>
-    <row r="88" ht="15" customHeight="1">
-      <c r="A88" t="s" s="12">
+      <c r="D88" s="5"/>
+      <c r="E88" s="6"/>
+    </row>
+    <row r="89" spans="1:5" ht="15" customHeight="1">
+      <c r="A89" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="B88" t="s" s="13">
+      <c r="B89" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C88" t="s" s="14">
+      <c r="C89" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D88" s="7"/>
-      <c r="E88" s="8"/>
-    </row>
-    <row r="89" ht="15" customHeight="1">
-      <c r="A89" t="s" s="12">
+      <c r="D89" s="5"/>
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" spans="1:5" ht="15" customHeight="1">
+      <c r="A90" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B89" t="s" s="13">
+      <c r="B90" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C89" t="s" s="14">
+      <c r="C90" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="7"/>
-      <c r="E89" s="8"/>
-    </row>
-    <row r="90" ht="15" customHeight="1">
-      <c r="A90" t="s" s="12">
+      <c r="D90" s="5"/>
+      <c r="E90" s="6"/>
+    </row>
+    <row r="91" spans="1:5" ht="15" customHeight="1">
+      <c r="A91" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="B90" t="s" s="13">
+      <c r="B91" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C90" t="s" s="14">
+      <c r="C91" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D90" s="7"/>
-      <c r="E90" s="8"/>
-    </row>
-    <row r="91" ht="15" customHeight="1">
-      <c r="A91" t="s" s="12">
+      <c r="D91" s="5"/>
+      <c r="E91" s="6"/>
+    </row>
+    <row r="92" spans="1:5" ht="15" customHeight="1">
+      <c r="A92" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="B91" t="s" s="13">
+      <c r="B92" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C91" t="s" s="14">
+      <c r="C92" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="D91" s="7"/>
-      <c r="E91" s="8"/>
-    </row>
-    <row r="92" ht="15" customHeight="1">
-      <c r="A92" t="s" s="12">
+      <c r="D92" s="5"/>
+      <c r="E92" s="6"/>
+    </row>
+    <row r="93" spans="1:5" ht="15" customHeight="1">
+      <c r="A93" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="B92" t="s" s="13">
+      <c r="B93" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C92" t="s" s="14">
+      <c r="C93" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D92" s="7"/>
-      <c r="E92" s="8"/>
-    </row>
-    <row r="93" ht="15" customHeight="1">
-      <c r="A93" t="s" s="12">
+      <c r="D93" s="5"/>
+      <c r="E93" s="6"/>
+    </row>
+    <row r="94" spans="1:5" ht="15" customHeight="1">
+      <c r="A94" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="B93" t="s" s="13">
+      <c r="B94" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C93" t="s" s="14">
+      <c r="C94" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D93" s="7"/>
-      <c r="E93" s="8"/>
-    </row>
-    <row r="94" ht="15" customHeight="1">
-      <c r="A94" t="s" s="12">
+      <c r="D94" s="5"/>
+      <c r="E94" s="6"/>
+    </row>
+    <row r="95" spans="1:5" ht="15" customHeight="1">
+      <c r="A95" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="B94" t="s" s="13">
+      <c r="B95" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C94" t="s" s="14">
+      <c r="C95" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D94" s="7"/>
-      <c r="E94" s="8"/>
-    </row>
-    <row r="95" ht="15" customHeight="1">
-      <c r="A95" t="s" s="12">
+      <c r="D95" s="5"/>
+      <c r="E95" s="6"/>
+    </row>
+    <row r="96" spans="1:5" ht="15" customHeight="1">
+      <c r="A96" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="B95" t="s" s="13">
+      <c r="B96" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C95" t="s" s="14">
+      <c r="C96" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D95" s="7"/>
-      <c r="E95" s="8"/>
-    </row>
-    <row r="96" ht="15" customHeight="1">
-      <c r="A96" t="s" s="12">
+      <c r="D96" s="5"/>
+      <c r="E96" s="6"/>
+    </row>
+    <row r="97" spans="1:5" ht="15" customHeight="1">
+      <c r="A97" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="B96" t="s" s="13">
+      <c r="B97" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C96" t="s" s="14">
+      <c r="C97" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D96" s="7"/>
-      <c r="E96" s="8"/>
-    </row>
-    <row r="97" ht="15" customHeight="1">
-      <c r="A97" t="s" s="12">
+      <c r="D97" s="5"/>
+      <c r="E97" s="6"/>
+    </row>
+    <row r="98" spans="1:5" ht="15" customHeight="1">
+      <c r="A98" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="B97" t="s" s="13">
+      <c r="B98" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C97" t="s" s="14">
+      <c r="C98" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="D97" s="7"/>
-      <c r="E97" s="8"/>
-    </row>
-    <row r="98" ht="15" customHeight="1">
-      <c r="A98" t="s" s="12">
+      <c r="D98" s="5"/>
+      <c r="E98" s="6"/>
+    </row>
+    <row r="99" spans="1:5" ht="15" customHeight="1">
+      <c r="A99" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B98" t="s" s="13">
+      <c r="B99" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C98" t="s" s="14">
+      <c r="C99" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D98" s="7"/>
-      <c r="E98" s="8"/>
-    </row>
-    <row r="99" ht="27" customHeight="1">
-      <c r="A99" t="s" s="12">
+      <c r="D99" s="5"/>
+      <c r="E99" s="6"/>
+    </row>
+    <row r="100" spans="1:5" ht="27" customHeight="1">
+      <c r="A100" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="B99" t="s" s="13">
+      <c r="B100" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C99" t="s" s="14">
+      <c r="C100" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="D99" s="7"/>
-      <c r="E99" s="8"/>
-    </row>
-    <row r="100" ht="27" customHeight="1">
-      <c r="A100" t="s" s="12">
+      <c r="D100" s="5"/>
+      <c r="E100" s="6"/>
+    </row>
+    <row r="101" spans="1:5" ht="27" customHeight="1">
+      <c r="A101" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="B100" t="s" s="13">
+      <c r="B101" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C100" t="s" s="14">
+      <c r="C101" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="D100" s="7"/>
-      <c r="E100" s="8"/>
-    </row>
-    <row r="101" ht="27" customHeight="1">
-      <c r="A101" t="s" s="12">
+      <c r="D101" s="5"/>
+      <c r="E101" s="6"/>
+    </row>
+    <row r="102" spans="1:5" ht="27" customHeight="1">
+      <c r="A102" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="B101" t="s" s="13">
+      <c r="B102" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C101" t="s" s="14">
+      <c r="C102" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="D101" s="7"/>
-      <c r="E101" s="8"/>
-    </row>
-    <row r="102" ht="39" customHeight="1">
-      <c r="A102" t="s" s="12">
+      <c r="D102" s="5"/>
+      <c r="E102" s="6"/>
+    </row>
+    <row r="103" spans="1:5" ht="39" customHeight="1">
+      <c r="A103" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="B102" t="s" s="13">
+      <c r="B103" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C102" t="s" s="14">
+      <c r="C103" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="D102" s="7"/>
-      <c r="E102" s="8"/>
-    </row>
-    <row r="103" ht="15" customHeight="1">
-      <c r="A103" t="s" s="12">
+      <c r="D103" s="5"/>
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="1:5" ht="15" customHeight="1">
+      <c r="A104" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="B103" t="s" s="13">
+      <c r="B104" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C103" t="s" s="14">
+      <c r="C104" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="D103" s="7"/>
-      <c r="E103" s="8"/>
-    </row>
-    <row r="104" ht="15" customHeight="1">
-      <c r="A104" t="s" s="12">
+      <c r="D104" s="5"/>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="1:5" ht="15" customHeight="1">
+      <c r="A105" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="B104" t="s" s="13">
+      <c r="B105" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C104" t="s" s="14">
+      <c r="C105" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="D104" s="7"/>
-      <c r="E104" s="8"/>
-    </row>
-    <row r="105" ht="15" customHeight="1">
-      <c r="A105" t="s" s="12">
+      <c r="D105" s="5"/>
+      <c r="E105" s="6"/>
+    </row>
+    <row r="106" spans="1:5" ht="15" customHeight="1">
+      <c r="A106" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="B105" t="s" s="13">
+      <c r="B106" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C105" t="s" s="14">
+      <c r="C106" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="D105" s="7"/>
-      <c r="E105" s="8"/>
-    </row>
-    <row r="106" ht="15" customHeight="1">
-      <c r="A106" t="s" s="12">
+      <c r="D106" s="5"/>
+      <c r="E106" s="6"/>
+    </row>
+    <row r="107" spans="1:5" ht="15" customHeight="1">
+      <c r="A107" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="B106" t="s" s="13">
+      <c r="B107" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C106" t="s" s="14">
+      <c r="C107" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="D106" s="7"/>
-      <c r="E106" s="8"/>
-    </row>
-    <row r="107" ht="27" customHeight="1">
-      <c r="A107" t="s" s="12">
+      <c r="D107" s="5"/>
+      <c r="E107" s="6"/>
+    </row>
+    <row r="108" spans="1:5" ht="27" customHeight="1">
+      <c r="A108" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B107" t="s" s="13">
+      <c r="B108" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C107" t="s" s="14">
+      <c r="C108" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D107" s="7"/>
-      <c r="E107" s="8"/>
-    </row>
-    <row r="108" ht="27" customHeight="1">
-      <c r="A108" t="s" s="12">
+      <c r="D108" s="5"/>
+      <c r="E108" s="6"/>
+    </row>
+    <row r="109" spans="1:5" ht="27" customHeight="1">
+      <c r="A109" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="B108" t="s" s="13">
+      <c r="B109" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C108" t="s" s="14">
+      <c r="C109" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D108" s="7"/>
-      <c r="E108" s="8"/>
-    </row>
-    <row r="109" ht="15" customHeight="1">
-      <c r="A109" t="s" s="12">
+      <c r="D109" s="5"/>
+      <c r="E109" s="6"/>
+    </row>
+    <row r="110" spans="1:5" ht="15" customHeight="1">
+      <c r="A110" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="B109" t="s" s="13">
+      <c r="B110" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C109" t="s" s="14">
+      <c r="C110" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D109" s="7"/>
-      <c r="E109" s="8"/>
-    </row>
-    <row r="110" ht="27" customHeight="1">
-      <c r="A110" t="s" s="12">
+      <c r="D110" s="5"/>
+      <c r="E110" s="6"/>
+    </row>
+    <row r="111" spans="1:5" ht="27" customHeight="1">
+      <c r="A111" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="B110" t="s" s="13">
+      <c r="B111" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C110" t="s" s="14">
+      <c r="C111" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D110" s="7"/>
-      <c r="E110" s="8"/>
-    </row>
-    <row r="111" ht="15" customHeight="1">
-      <c r="A111" t="s" s="12">
+      <c r="D111" s="5"/>
+      <c r="E111" s="6"/>
+    </row>
+    <row r="112" spans="1:5" ht="15" customHeight="1">
+      <c r="A112" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="B111" t="s" s="13">
+      <c r="B112" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C111" t="s" s="14">
+      <c r="C112" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="D111" s="7"/>
-      <c r="E111" s="8"/>
-    </row>
-    <row r="112" ht="15" customHeight="1">
-      <c r="A112" t="s" s="12">
+      <c r="D112" s="5"/>
+      <c r="E112" s="6"/>
+    </row>
+    <row r="113" spans="1:5" ht="15" customHeight="1">
+      <c r="A113" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="B112" t="s" s="13">
+      <c r="B113" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C112" t="s" s="14">
+      <c r="C113" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="D112" s="7"/>
-      <c r="E112" s="8"/>
-    </row>
-    <row r="113" ht="27" customHeight="1">
-      <c r="A113" t="s" s="12">
+      <c r="D113" s="5"/>
+      <c r="E113" s="6"/>
+    </row>
+    <row r="114" spans="1:5" ht="27" customHeight="1">
+      <c r="A114" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B113" t="s" s="13">
+      <c r="B114" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C113" t="s" s="14">
+      <c r="C114" s="12" t="s">
         <v>231</v>
       </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="8"/>
-    </row>
-    <row r="114" ht="15" customHeight="1">
-      <c r="A114" t="s" s="12">
+      <c r="D114" s="5"/>
+      <c r="E114" s="6"/>
+    </row>
+    <row r="115" spans="1:5" ht="15" customHeight="1">
+      <c r="A115" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="B114" t="s" s="13">
+      <c r="B115" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C114" t="s" s="14">
+      <c r="C115" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="D114" s="7"/>
-      <c r="E114" s="8"/>
-    </row>
-    <row r="115" ht="27" customHeight="1">
-      <c r="A115" t="s" s="12">
+      <c r="D115" s="5"/>
+      <c r="E115" s="6"/>
+    </row>
+    <row r="116" spans="1:5" ht="27" customHeight="1">
+      <c r="A116" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="B115" t="s" s="13">
+      <c r="B116" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C115" t="s" s="14">
+      <c r="C116" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="D115" s="7"/>
-      <c r="E115" s="8"/>
-    </row>
-    <row r="116" ht="27" customHeight="1">
-      <c r="A116" t="s" s="12">
+      <c r="D116" s="5"/>
+      <c r="E116" s="6"/>
+    </row>
+    <row r="117" spans="1:5" ht="27" customHeight="1">
+      <c r="A117" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="B116" t="s" s="13">
+      <c r="B117" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C116" t="s" s="14">
+      <c r="C117" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="D116" s="7"/>
-      <c r="E116" s="8"/>
-    </row>
-    <row r="117" ht="15" customHeight="1">
-      <c r="A117" t="s" s="12">
+      <c r="D117" s="5"/>
+      <c r="E117" s="6"/>
+    </row>
+    <row r="118" spans="1:5" ht="15" customHeight="1">
+      <c r="A118" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="B117" t="s" s="13">
+      <c r="B118" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C117" t="s" s="14">
+      <c r="C118" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="D117" s="7"/>
-      <c r="E117" s="8"/>
-    </row>
-    <row r="118" ht="15" customHeight="1">
-      <c r="A118" t="s" s="12">
+      <c r="D118" s="5"/>
+      <c r="E118" s="6"/>
+    </row>
+    <row r="119" spans="1:5" ht="15" customHeight="1">
+      <c r="A119" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="B118" t="s" s="13">
+      <c r="B119" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C118" t="s" s="14">
+      <c r="C119" s="12" t="s">
         <v>241</v>
       </c>
-      <c r="D118" s="7"/>
-      <c r="E118" s="8"/>
-    </row>
-    <row r="119" ht="15" customHeight="1">
-      <c r="A119" t="s" s="12">
+      <c r="D119" s="5"/>
+      <c r="E119" s="6"/>
+    </row>
+    <row r="120" spans="1:5" ht="15" customHeight="1">
+      <c r="A120" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="B119" t="s" s="13">
+      <c r="B120" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C119" t="s" s="14">
+      <c r="C120" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="D119" s="7"/>
-      <c r="E119" s="8"/>
-    </row>
-    <row r="120" ht="15" customHeight="1">
-      <c r="A120" t="s" s="12">
+      <c r="D120" s="5"/>
+      <c r="E120" s="6"/>
+    </row>
+    <row r="121" spans="1:5" ht="15" customHeight="1">
+      <c r="A121" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="B120" t="s" s="13">
+      <c r="B121" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C120" t="s" s="14">
+      <c r="C121" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="D120" s="7"/>
-      <c r="E120" s="8"/>
-    </row>
-    <row r="121" ht="27" customHeight="1">
-      <c r="A121" t="s" s="12">
+      <c r="D121" s="5"/>
+      <c r="E121" s="6"/>
+    </row>
+    <row r="122" spans="1:5" ht="27" customHeight="1">
+      <c r="A122" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="B121" t="s" s="13">
+      <c r="B122" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C121" t="s" s="14">
+      <c r="C122" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="D121" s="7"/>
-      <c r="E121" s="8"/>
-    </row>
-    <row r="122" ht="27" customHeight="1">
-      <c r="A122" t="s" s="12">
+      <c r="D122" s="5"/>
+      <c r="E122" s="6"/>
+    </row>
+    <row r="123" spans="1:5" ht="27" customHeight="1">
+      <c r="A123" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="B122" t="s" s="13">
+      <c r="B123" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C122" t="s" s="14">
+      <c r="C123" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D122" s="7"/>
-      <c r="E122" s="8"/>
-    </row>
-    <row r="123" ht="15" customHeight="1">
-      <c r="A123" t="s" s="12">
+      <c r="D123" s="5"/>
+      <c r="E123" s="6"/>
+    </row>
+    <row r="124" spans="1:5" ht="15" customHeight="1">
+      <c r="A124" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="B123" t="s" s="13">
+      <c r="B124" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="C123" t="s" s="14">
+      <c r="C124" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="D123" s="7"/>
-      <c r="E123" s="8"/>
-    </row>
-    <row r="124" ht="27" customHeight="1">
-      <c r="A124" t="s" s="12">
+      <c r="D124" s="5"/>
+      <c r="E124" s="6"/>
+    </row>
+    <row r="125" spans="1:5" ht="27" customHeight="1">
+      <c r="A125" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="B124" t="s" s="13">
+      <c r="B125" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C124" t="s" s="14">
+      <c r="C125" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="D124" s="7"/>
-      <c r="E124" s="8"/>
-    </row>
-    <row r="125" ht="27" customHeight="1">
-      <c r="A125" t="s" s="12">
+      <c r="D125" s="5"/>
+      <c r="E125" s="6"/>
+    </row>
+    <row r="126" spans="1:5" ht="27" customHeight="1">
+      <c r="A126" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="B125" t="s" s="13">
+      <c r="B126" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C125" t="s" s="14">
+      <c r="C126" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="D125" s="7"/>
-      <c r="E125" s="8"/>
-    </row>
-    <row r="126" ht="15" customHeight="1">
-      <c r="A126" t="s" s="12">
+      <c r="D126" s="5"/>
+      <c r="E126" s="6"/>
+    </row>
+    <row r="127" spans="1:5" ht="15" customHeight="1">
+      <c r="A127" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="B126" t="s" s="13">
+      <c r="B127" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C126" t="s" s="14">
+      <c r="C127" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="D126" s="7"/>
-      <c r="E126" s="8"/>
-    </row>
-    <row r="127" ht="27" customHeight="1">
-      <c r="A127" t="s" s="12">
+      <c r="D127" s="5"/>
+      <c r="E127" s="6"/>
+    </row>
+    <row r="128" spans="1:5" ht="27" customHeight="1">
+      <c r="A128" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="B127" t="s" s="13">
+      <c r="B128" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C127" t="s" s="14">
+      <c r="C128" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="D127" s="7"/>
-      <c r="E127" s="8"/>
-    </row>
-    <row r="128" ht="27" customHeight="1">
-      <c r="A128" t="s" s="12">
+      <c r="D128" s="5"/>
+      <c r="E128" s="6"/>
+    </row>
+    <row r="129" spans="1:5" ht="27" customHeight="1">
+      <c r="A129" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="B128" t="s" s="13">
+      <c r="B129" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C128" t="s" s="14">
+      <c r="C129" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="D128" s="7"/>
-      <c r="E128" s="8"/>
-    </row>
-    <row r="129" ht="27" customHeight="1">
-      <c r="A129" t="s" s="12">
+      <c r="D129" s="5"/>
+      <c r="E129" s="6"/>
+    </row>
+    <row r="130" spans="1:5" ht="27" customHeight="1">
+      <c r="A130" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="B129" t="s" s="13">
+      <c r="B130" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C129" t="s" s="14">
+      <c r="C130" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="D129" s="7"/>
-      <c r="E129" s="8"/>
-    </row>
-    <row r="130" ht="27" customHeight="1">
-      <c r="A130" t="s" s="12">
+      <c r="D130" s="5"/>
+      <c r="E130" s="6"/>
+    </row>
+    <row r="131" spans="1:5" ht="27" customHeight="1">
+      <c r="A131" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="B130" t="s" s="13">
+      <c r="B131" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C130" t="s" s="14">
+      <c r="C131" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="D130" s="7"/>
-      <c r="E130" s="8"/>
-    </row>
-    <row r="131" ht="27" customHeight="1">
-      <c r="A131" t="s" s="12">
+      <c r="D131" s="5"/>
+      <c r="E131" s="6"/>
+    </row>
+    <row r="132" spans="1:5" ht="27" customHeight="1">
+      <c r="A132" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="B131" t="s" s="13">
+      <c r="B132" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C131" t="s" s="14">
+      <c r="C132" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="D131" s="20"/>
-      <c r="E131" s="21"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update and align experiment data compilation with new mock data
- Update extract_sart_blocks() to account for additional post-block question
- Improve summarize_sart_chunk() and compile_experiment_data()
</commit_message>
<xml_diff>
--- a/data/variable-legend.xlsx
+++ b/data/variable-legend.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="295">
   <si>
     <t>Table 1</t>
   </si>
@@ -832,6 +832,78 @@
   </si>
   <si>
     <t>Boredom rating prior to experiment</t>
+  </si>
+  <si>
+    <t>blkN_boredom</t>
+  </si>
+  <si>
+    <t>Block boredom rating</t>
+  </si>
+  <si>
+    <t>avg_boredom</t>
+  </si>
+  <si>
+    <t>Average block boredom rating</t>
+  </si>
+  <si>
+    <t>auc_boredom</t>
+  </si>
+  <si>
+    <t>Area under the curve calculation for block boredom ratings</t>
+  </si>
+  <si>
+    <t>end_boredom</t>
+  </si>
+  <si>
+    <t>Boredom rating for the last block</t>
+  </si>
+  <si>
+    <t>peak_boredom</t>
+  </si>
+  <si>
+    <t>Peak (maximum) boredom rating</t>
+  </si>
+  <si>
+    <t>min_boredom</t>
+  </si>
+  <si>
+    <t>Minimum boredom rating</t>
+  </si>
+  <si>
+    <t>prop_boredom_downs</t>
+  </si>
+  <si>
+    <t>prop_boredom_sames</t>
+  </si>
+  <si>
+    <t>prop_boredomt_ups</t>
+  </si>
+  <si>
+    <t>Proportion of boredom ratings that increased from the previous boredom rating</t>
+  </si>
+  <si>
+    <t>Proportion of boredom ratings that held steady with the previous boredom rating</t>
+  </si>
+  <si>
+    <t>Proportion of boredom ratings that dropped from the previous boredom rating</t>
+  </si>
+  <si>
+    <t>boredom_intercept</t>
+  </si>
+  <si>
+    <t>boredom_slope</t>
+  </si>
+  <si>
+    <t>Linear regression slope for boredom ratings</t>
+  </si>
+  <si>
+    <t>Linear regression intercept for boredom ratings</t>
+  </si>
+  <si>
+    <t>start_boredom</t>
+  </si>
+  <si>
+    <t>Boredom rating for the first block</t>
   </si>
 </sst>
 </file>
@@ -1127,8 +1199,62 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1206,9 +1332,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2392,10 +2536,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV132"/>
+  <dimension ref="A1:IV144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -2597,12 +2741,12 @@
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+    <row r="18" spans="1:5" ht="27" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>36</v>
+        <v>275</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>37</v>
+        <v>276</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="5"/>
@@ -2610,21 +2754,21 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" ht="27" customHeight="1">
+    <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="5"/>
@@ -2632,47 +2776,47 @@
     </row>
     <row r="21" spans="1:5" ht="27" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>44</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C21" s="12"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
+    <row r="22" spans="1:5" ht="27" customHeight="1">
       <c r="A22" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="5"/>
@@ -2680,10 +2824,10 @@
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="5"/>
@@ -2691,10 +2835,10 @@
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="10" t="s">
-        <v>54</v>
+        <v>273</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>55</v>
+        <v>274</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="5"/>
@@ -2702,10 +2846,10 @@
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="A27" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="5"/>
@@ -2713,10 +2857,10 @@
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
       <c r="A28" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="5"/>
@@ -2724,10 +2868,10 @@
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1">
       <c r="A29" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="5"/>
@@ -2735,10 +2879,10 @@
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1">
       <c r="A30" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="5"/>
@@ -2746,45 +2890,43 @@
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>63</v>
+        <v>271</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>64</v>
+        <v>272</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:5" ht="27" customHeight="1">
+    <row r="32" spans="1:5" ht="15" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>67</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C32" s="12"/>
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
     </row>
-    <row r="33" spans="1:5" ht="27" customHeight="1">
+    <row r="33" spans="1:5" ht="15" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="13"/>
+        <v>62</v>
+      </c>
+      <c r="C33" s="12"/>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" ht="27" customHeight="1">
+    <row r="34" spans="1:5" ht="15" customHeight="1">
       <c r="A34" s="10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="5"/>
@@ -2792,10 +2934,10 @@
     </row>
     <row r="35" spans="1:5" ht="27" customHeight="1">
       <c r="A35" s="10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>67</v>
@@ -2803,45 +2945,47 @@
       <c r="D35" s="5"/>
       <c r="E35" s="6"/>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1">
+    <row r="36" spans="1:5" ht="27" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="C36" s="13"/>
       <c r="D36" s="5"/>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1">
+    <row r="37" spans="1:5" ht="27" customHeight="1">
       <c r="A37" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="5"/>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1">
+    <row r="38" spans="1:5" ht="27" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="12"/>
+        <v>73</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="5"/>
@@ -2849,10 +2993,10 @@
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="5"/>
@@ -2860,10 +3004,10 @@
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="5"/>
@@ -2871,10 +3015,10 @@
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="5"/>
@@ -2882,10 +3026,10 @@
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="5"/>
@@ -2893,10 +3037,10 @@
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1">
       <c r="A44" s="10" t="s">
-        <v>90</v>
+        <v>277</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>91</v>
+        <v>278</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="5"/>
@@ -2904,10 +3048,10 @@
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1">
       <c r="A45" s="10" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C45" s="12"/>
       <c r="D45" s="5"/>
@@ -2915,10 +3059,10 @@
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1">
       <c r="A46" s="10" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C46" s="12"/>
       <c r="D46" s="5"/>
@@ -2926,10 +3070,10 @@
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1">
       <c r="A47" s="10" t="s">
-        <v>269</v>
+        <v>88</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>270</v>
+        <v>89</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="5"/>
@@ -2937,10 +3081,10 @@
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
       <c r="A48" s="10" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="5"/>
@@ -2948,32 +3092,32 @@
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1">
       <c r="A49" s="10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="5"/>
       <c r="E49" s="6"/>
     </row>
-    <row r="50" spans="1:5" ht="27" customHeight="1">
+    <row r="50" spans="1:5" ht="15" customHeight="1">
       <c r="A50" s="10" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
     </row>
-    <row r="51" spans="1:5" ht="27" customHeight="1">
+    <row r="51" spans="1:5" ht="15" customHeight="1">
       <c r="A51" s="10" t="s">
-        <v>102</v>
+        <v>269</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>103</v>
+        <v>270</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="5"/>
@@ -2981,10 +3125,10 @@
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1">
       <c r="A52" s="10" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="5"/>
@@ -2992,1005 +3136,1139 @@
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
       <c r="A53" s="10" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C53" s="12"/>
       <c r="D53" s="5"/>
       <c r="E53" s="6"/>
     </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1">
+    <row r="54" spans="1:5" ht="27" customHeight="1">
       <c r="A54" s="10" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>108</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C54" s="12"/>
       <c r="D54" s="5"/>
       <c r="E54" s="6"/>
     </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1">
+    <row r="55" spans="1:5" ht="27" customHeight="1">
       <c r="A55" s="10" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="15"/>
+        <v>103</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="5"/>
       <c r="E55" s="6"/>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1">
       <c r="A56" s="10" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="5"/>
       <c r="E56" s="6"/>
     </row>
-    <row r="57" spans="1:5" ht="27" customHeight="1">
+    <row r="57" spans="1:5" ht="15" customHeight="1">
       <c r="A57" s="10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C57" s="12"/>
+        <v>107</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="D57" s="5"/>
       <c r="E57" s="6"/>
     </row>
-    <row r="58" spans="1:5" ht="27" customHeight="1">
+    <row r="58" spans="1:5" ht="15" customHeight="1">
       <c r="A58" s="10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C58" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="D58" s="5"/>
       <c r="E58" s="6"/>
     </row>
-    <row r="59" spans="1:5" ht="27" customHeight="1">
+    <row r="59" spans="1:5" ht="15" customHeight="1">
       <c r="A59" s="10" t="s">
-        <v>119</v>
+        <v>279</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="12"/>
+        <v>280</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>108</v>
+      </c>
       <c r="D59" s="5"/>
       <c r="E59" s="6"/>
     </row>
-    <row r="60" spans="1:5" ht="27" customHeight="1">
+    <row r="60" spans="1:5" ht="15" customHeight="1">
       <c r="A60" s="10" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="5"/>
+        <v>112</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="15"/>
       <c r="E60" s="6"/>
     </row>
-    <row r="61" spans="1:5" ht="27" customHeight="1">
+    <row r="61" spans="1:5" ht="15" customHeight="1">
       <c r="A61" s="10" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C61" s="12"/>
       <c r="D61" s="5"/>
       <c r="E61" s="6"/>
     </row>
-    <row r="62" spans="1:5" ht="27" customHeight="1">
+    <row r="62" spans="1:5" ht="15" customHeight="1">
       <c r="A62" s="10" t="s">
-        <v>125</v>
+        <v>281</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>126</v>
+        <v>282</v>
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="5"/>
       <c r="E62" s="6"/>
     </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1">
+    <row r="63" spans="1:5" ht="27" customHeight="1">
       <c r="A63" s="10" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C63" s="12"/>
       <c r="D63" s="5"/>
       <c r="E63" s="6"/>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1">
+    <row r="64" spans="1:5" ht="27" customHeight="1">
       <c r="A64" s="10" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C64" s="12"/>
       <c r="D64" s="5"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1">
+    <row r="65" spans="1:5" ht="27" customHeight="1">
       <c r="A65" s="10" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C65" s="12"/>
       <c r="D65" s="5"/>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1">
+    <row r="66" spans="1:5" ht="27" customHeight="1">
       <c r="A66" s="10" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C66" s="12"/>
       <c r="D66" s="5"/>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1">
+    <row r="67" spans="1:5" ht="27" customHeight="1">
       <c r="A67" s="10" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C67" s="12"/>
       <c r="D67" s="5"/>
       <c r="E67" s="6"/>
     </row>
-    <row r="68" spans="1:5" ht="15" customHeight="1">
+    <row r="68" spans="1:5" ht="27" customHeight="1">
       <c r="A68" s="10" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C68" s="12"/>
       <c r="D68" s="5"/>
       <c r="E68" s="6"/>
     </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1">
+    <row r="69" spans="1:5" ht="27" customHeight="1">
       <c r="A69" s="10" t="s">
-        <v>139</v>
+        <v>283</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>140</v>
+        <v>288</v>
       </c>
       <c r="C69" s="12"/>
       <c r="D69" s="5"/>
       <c r="E69" s="6"/>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1">
+    <row r="70" spans="1:5" ht="27" customHeight="1">
       <c r="A70" s="10" t="s">
-        <v>141</v>
+        <v>284</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>142</v>
+        <v>287</v>
       </c>
       <c r="C70" s="12"/>
       <c r="D70" s="5"/>
       <c r="E70" s="6"/>
     </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1">
+    <row r="71" spans="1:5" ht="27" customHeight="1">
       <c r="A71" s="10" t="s">
-        <v>143</v>
+        <v>285</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>144</v>
+        <v>286</v>
       </c>
       <c r="C71" s="12"/>
       <c r="D71" s="5"/>
       <c r="E71" s="6"/>
     </row>
-    <row r="72" spans="1:5" ht="27" customHeight="1">
+    <row r="72" spans="1:5" ht="15" customHeight="1">
       <c r="A72" s="10" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C72" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C72" s="12"/>
       <c r="D72" s="5"/>
       <c r="E72" s="6"/>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1">
       <c r="A73" s="10" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C73" s="12"/>
       <c r="D73" s="5"/>
       <c r="E73" s="6"/>
     </row>
-    <row r="74" spans="1:5" ht="27" customHeight="1">
+    <row r="74" spans="1:5" ht="15" customHeight="1">
       <c r="A74" s="10" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C74" s="12"/>
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1">
       <c r="A75" s="10" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C75" s="12"/>
       <c r="D75" s="5"/>
       <c r="E75" s="6"/>
     </row>
     <row r="76" spans="1:5" ht="15" customHeight="1">
       <c r="A76" s="10" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C76" s="12"/>
       <c r="D76" s="5"/>
       <c r="E76" s="6"/>
     </row>
     <row r="77" spans="1:5" ht="15" customHeight="1">
       <c r="A77" s="10" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="C77" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C77" s="12"/>
       <c r="D77" s="5"/>
       <c r="E77" s="6"/>
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1">
       <c r="A78" s="10" t="s">
-        <v>158</v>
+        <v>290</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C78" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="C78" s="12"/>
       <c r="D78" s="5"/>
       <c r="E78" s="6"/>
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1">
       <c r="A79" s="10" t="s">
-        <v>160</v>
+        <v>289</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="C79" s="12" t="s">
-        <v>147</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="C79" s="12"/>
       <c r="D79" s="5"/>
       <c r="E79" s="6"/>
     </row>
     <row r="80" spans="1:5" ht="15" customHeight="1">
       <c r="A80" s="10" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C80" s="13"/>
+        <v>140</v>
+      </c>
+      <c r="C80" s="12"/>
       <c r="D80" s="5"/>
       <c r="E80" s="6"/>
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1">
       <c r="A81" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="B81" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>165</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C81" s="12"/>
       <c r="D81" s="5"/>
       <c r="E81" s="6"/>
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1">
       <c r="A82" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C82" s="17"/>
+        <v>143</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C82" s="12"/>
       <c r="D82" s="5"/>
       <c r="E82" s="6"/>
     </row>
     <row r="83" spans="1:5" ht="15" customHeight="1">
       <c r="A83" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B83" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>168</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C83" s="12"/>
       <c r="D83" s="5"/>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" spans="1:5" ht="15" customHeight="1">
+    <row r="84" spans="1:5" ht="27" customHeight="1">
       <c r="A84" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B84" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="C84" s="11" t="s">
-        <v>170</v>
+        <v>145</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="D84" s="5"/>
       <c r="E84" s="6"/>
     </row>
     <row r="85" spans="1:5" ht="15" customHeight="1">
       <c r="A85" s="10" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C85" s="12" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="D85" s="5"/>
       <c r="E85" s="6"/>
     </row>
-    <row r="86" spans="1:5" ht="15" customHeight="1">
+    <row r="86" spans="1:5" ht="27" customHeight="1">
       <c r="A86" s="10" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="D86" s="5"/>
       <c r="E86" s="6"/>
     </row>
     <row r="87" spans="1:5" ht="15" customHeight="1">
       <c r="A87" s="10" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="D87" s="5"/>
       <c r="E87" s="6"/>
     </row>
     <row r="88" spans="1:5" ht="15" customHeight="1">
       <c r="A88" s="10" t="s">
-        <v>177</v>
+        <v>154</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="D88" s="5"/>
       <c r="E88" s="6"/>
     </row>
     <row r="89" spans="1:5" ht="15" customHeight="1">
       <c r="A89" s="10" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="6"/>
     </row>
     <row r="90" spans="1:5" ht="15" customHeight="1">
       <c r="A90" s="10" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="D90" s="5"/>
       <c r="E90" s="6"/>
     </row>
     <row r="91" spans="1:5" ht="15" customHeight="1">
       <c r="A91" s="10" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="D91" s="5"/>
       <c r="E91" s="6"/>
     </row>
     <row r="92" spans="1:5" ht="15" customHeight="1">
       <c r="A92" s="10" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="B92" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="C92" s="12" t="s">
-        <v>186</v>
-      </c>
+      <c r="C92" s="13"/>
       <c r="D92" s="5"/>
       <c r="E92" s="6"/>
     </row>
     <row r="93" spans="1:5" ht="15" customHeight="1">
       <c r="A93" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B93" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C93" s="12" t="s">
-        <v>188</v>
+      <c r="C93" s="11" t="s">
+        <v>165</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="6"/>
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1">
       <c r="A94" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="B94" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C94" s="12" t="s">
-        <v>190</v>
-      </c>
+      <c r="C94" s="17"/>
       <c r="D94" s="5"/>
       <c r="E94" s="6"/>
     </row>
     <row r="95" spans="1:5" ht="15" customHeight="1">
       <c r="A95" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="B95" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B95" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C95" s="12" t="s">
-        <v>192</v>
+      <c r="C95" s="11" t="s">
+        <v>168</v>
       </c>
       <c r="D95" s="5"/>
       <c r="E95" s="6"/>
     </row>
     <row r="96" spans="1:5" ht="15" customHeight="1">
       <c r="A96" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="B96" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B96" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="C96" s="12" t="s">
-        <v>192</v>
+      <c r="C96" s="11" t="s">
+        <v>170</v>
       </c>
       <c r="D96" s="5"/>
       <c r="E96" s="6"/>
     </row>
     <row r="97" spans="1:5" ht="15" customHeight="1">
       <c r="A97" s="10" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="B97" s="11" t="s">
         <v>163</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="D97" s="5"/>
       <c r="E97" s="6"/>
     </row>
     <row r="98" spans="1:5" ht="15" customHeight="1">
       <c r="A98" s="10" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="B98" s="11" t="s">
         <v>163</v>
       </c>
       <c r="C98" s="12" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="D98" s="5"/>
       <c r="E98" s="6"/>
     </row>
     <row r="99" spans="1:5" ht="15" customHeight="1">
       <c r="A99" s="10" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="B99" s="11" t="s">
         <v>163</v>
       </c>
       <c r="C99" s="12" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="D99" s="5"/>
       <c r="E99" s="6"/>
     </row>
-    <row r="100" spans="1:5" ht="27" customHeight="1">
+    <row r="100" spans="1:5" ht="15" customHeight="1">
       <c r="A100" s="10" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C100" s="12" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="D100" s="5"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="1:5" ht="27" customHeight="1">
+    <row r="101" spans="1:5" ht="15" customHeight="1">
       <c r="A101" s="10" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C101" s="12" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="D101" s="5"/>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="1:5" ht="27" customHeight="1">
+    <row r="102" spans="1:5" ht="15" customHeight="1">
       <c r="A102" s="10" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C102" s="12" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
       <c r="D102" s="5"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="1:5" ht="39" customHeight="1">
+    <row r="103" spans="1:5" ht="15" customHeight="1">
       <c r="A103" s="10" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D103" s="5"/>
       <c r="E103" s="6"/>
     </row>
     <row r="104" spans="1:5" ht="15" customHeight="1">
       <c r="A104" s="10" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="B104" s="11" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C104" s="12" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="D104" s="5"/>
       <c r="E104" s="6"/>
     </row>
     <row r="105" spans="1:5" ht="15" customHeight="1">
       <c r="A105" s="10" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C105" s="12" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="D105" s="5"/>
       <c r="E105" s="6"/>
     </row>
     <row r="106" spans="1:5" ht="15" customHeight="1">
       <c r="A106" s="10" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="D106" s="5"/>
       <c r="E106" s="6"/>
     </row>
     <row r="107" spans="1:5" ht="15" customHeight="1">
       <c r="A107" s="10" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="D107" s="5"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="1:5" ht="27" customHeight="1">
+    <row r="108" spans="1:5" ht="15" customHeight="1">
       <c r="A108" s="10" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="D108" s="5"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:5" ht="27" customHeight="1">
+    <row r="109" spans="1:5" ht="15" customHeight="1">
       <c r="A109" s="10" t="s">
-        <v>220</v>
+        <v>194</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="D109" s="5"/>
       <c r="E109" s="6"/>
     </row>
     <row r="110" spans="1:5" ht="15" customHeight="1">
       <c r="A110" s="10" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>223</v>
+        <v>197</v>
       </c>
       <c r="D110" s="5"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:5" ht="27" customHeight="1">
+    <row r="111" spans="1:5" ht="15" customHeight="1">
       <c r="A111" s="10" t="s">
-        <v>224</v>
+        <v>198</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>225</v>
+        <v>199</v>
       </c>
       <c r="D111" s="5"/>
       <c r="E111" s="6"/>
     </row>
-    <row r="112" spans="1:5" ht="15" customHeight="1">
+    <row r="112" spans="1:5" ht="27" customHeight="1">
       <c r="A112" s="10" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="B112" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="D112" s="5"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="1:5" ht="15" customHeight="1">
+    <row r="113" spans="1:5" ht="27" customHeight="1">
       <c r="A113" s="10" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="D113" s="5"/>
       <c r="E113" s="6"/>
     </row>
     <row r="114" spans="1:5" ht="27" customHeight="1">
       <c r="A114" s="10" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="D114" s="5"/>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="1:5" ht="15" customHeight="1">
+    <row r="115" spans="1:5" ht="39" customHeight="1">
       <c r="A115" s="10" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="D115" s="5"/>
       <c r="E115" s="6"/>
     </row>
-    <row r="116" spans="1:5" ht="27" customHeight="1">
+    <row r="116" spans="1:5" ht="15" customHeight="1">
       <c r="A116" s="10" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="D116" s="5"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="1:5" ht="27" customHeight="1">
+    <row r="117" spans="1:5" ht="15" customHeight="1">
       <c r="A117" s="10" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="D117" s="5"/>
       <c r="E117" s="6"/>
     </row>
     <row r="118" spans="1:5" ht="15" customHeight="1">
       <c r="A118" s="10" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="D118" s="5"/>
       <c r="E118" s="6"/>
     </row>
     <row r="119" spans="1:5" ht="15" customHeight="1">
       <c r="A119" s="10" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="B119" s="11" t="s">
         <v>216</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="D119" s="5"/>
       <c r="E119" s="6"/>
     </row>
-    <row r="120" spans="1:5" ht="15" customHeight="1">
+    <row r="120" spans="1:5" ht="27" customHeight="1">
       <c r="A120" s="10" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="B120" s="11" t="s">
         <v>216</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D120" s="5"/>
       <c r="E120" s="6"/>
     </row>
-    <row r="121" spans="1:5" ht="15" customHeight="1">
+    <row r="121" spans="1:5" ht="27" customHeight="1">
       <c r="A121" s="10" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="B121" s="11" t="s">
         <v>216</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="D121" s="5"/>
       <c r="E121" s="6"/>
     </row>
-    <row r="122" spans="1:5" ht="27" customHeight="1">
+    <row r="122" spans="1:5" ht="15" customHeight="1">
       <c r="A122" s="10" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="B122" s="11" t="s">
         <v>216</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="D122" s="5"/>
       <c r="E122" s="6"/>
     </row>
     <row r="123" spans="1:5" ht="27" customHeight="1">
       <c r="A123" s="10" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="B123" s="11" t="s">
         <v>216</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="D123" s="5"/>
       <c r="E123" s="6"/>
     </row>
     <row r="124" spans="1:5" ht="15" customHeight="1">
       <c r="A124" s="10" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="B124" s="11" t="s">
         <v>216</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D124" s="5"/>
       <c r="E124" s="6"/>
     </row>
-    <row r="125" spans="1:5" ht="27" customHeight="1">
+    <row r="125" spans="1:5" ht="15" customHeight="1">
       <c r="A125" s="10" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="D125" s="5"/>
       <c r="E125" s="6"/>
     </row>
     <row r="126" spans="1:5" ht="27" customHeight="1">
       <c r="A126" s="10" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="D126" s="5"/>
       <c r="E126" s="6"/>
     </row>
     <row r="127" spans="1:5" ht="15" customHeight="1">
       <c r="A127" s="10" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="D127" s="5"/>
       <c r="E127" s="6"/>
     </row>
     <row r="128" spans="1:5" ht="27" customHeight="1">
       <c r="A128" s="10" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="D128" s="5"/>
       <c r="E128" s="6"/>
     </row>
     <row r="129" spans="1:5" ht="27" customHeight="1">
       <c r="A129" s="10" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="D129" s="5"/>
       <c r="E129" s="6"/>
     </row>
-    <row r="130" spans="1:5" ht="27" customHeight="1">
+    <row r="130" spans="1:5" ht="15" customHeight="1">
       <c r="A130" s="10" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="D130" s="5"/>
       <c r="E130" s="6"/>
     </row>
-    <row r="131" spans="1:5" ht="27" customHeight="1">
+    <row r="131" spans="1:5" ht="15" customHeight="1">
       <c r="A131" s="10" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="D131" s="5"/>
       <c r="E131" s="6"/>
     </row>
-    <row r="132" spans="1:5" ht="27" customHeight="1">
+    <row r="132" spans="1:5" ht="15" customHeight="1">
       <c r="A132" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B132" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D132" s="5"/>
+      <c r="E132" s="6"/>
+    </row>
+    <row r="133" spans="1:5" ht="15" customHeight="1">
+      <c r="A133" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D133" s="5"/>
+      <c r="E133" s="6"/>
+    </row>
+    <row r="134" spans="1:5" ht="27" customHeight="1">
+      <c r="A134" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="B134" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D134" s="5"/>
+      <c r="E134" s="6"/>
+    </row>
+    <row r="135" spans="1:5" ht="27" customHeight="1">
+      <c r="A135" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D135" s="5"/>
+      <c r="E135" s="6"/>
+    </row>
+    <row r="136" spans="1:5" ht="15" customHeight="1">
+      <c r="A136" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B136" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D136" s="5"/>
+      <c r="E136" s="6"/>
+    </row>
+    <row r="137" spans="1:5" ht="27" customHeight="1">
+      <c r="A137" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B137" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D137" s="5"/>
+      <c r="E137" s="6"/>
+    </row>
+    <row r="138" spans="1:5" ht="27" customHeight="1">
+      <c r="A138" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="B138" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D138" s="5"/>
+      <c r="E138" s="6"/>
+    </row>
+    <row r="139" spans="1:5" ht="15" customHeight="1">
+      <c r="A139" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="B139" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D139" s="5"/>
+      <c r="E139" s="6"/>
+    </row>
+    <row r="140" spans="1:5" ht="27" customHeight="1">
+      <c r="A140" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B140" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D140" s="5"/>
+      <c r="E140" s="6"/>
+    </row>
+    <row r="141" spans="1:5" ht="27" customHeight="1">
+      <c r="A141" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="B141" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D141" s="5"/>
+      <c r="E141" s="6"/>
+    </row>
+    <row r="142" spans="1:5" ht="27" customHeight="1">
+      <c r="A142" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="B142" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D142" s="5"/>
+      <c r="E142" s="6"/>
+    </row>
+    <row r="143" spans="1:5" ht="27" customHeight="1">
+      <c r="A143" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C143" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D143" s="5"/>
+      <c r="E143" s="6"/>
+    </row>
+    <row r="144" spans="1:5" ht="27" customHeight="1">
+      <c r="A144" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="B132" s="11" t="s">
+      <c r="B144" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="C132" s="12" t="s">
+      <c r="C144" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="D132" s="18"/>
-      <c r="E132" s="19"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>